<commit_message>
Added timings for Duplicates method
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -5,22 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissasedgwick/Projects/Makers/Week_9/algorithmic_complexity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissasedgwick/Projects/Makers/Week_10/algorithmic_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31B7D95-9FA6-3A42-BBD0-FA1FD3F009C9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC7D9EE-60B9-D749-B916-131FFCEEBCE6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-10960" windowWidth="38400" windowHeight="21600" xr2:uid="{0EC00D74-CF7F-6E46-A448-9AC86E039AD3}"/>
+    <workbookView xWindow="-38420" yWindow="-10500" windowWidth="38400" windowHeight="21140" xr2:uid="{0EC00D74-CF7F-6E46-A448-9AC86E039AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Graphs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Data!$S$47:$S$51</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Data!$T$47:$T$51</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Data!$S$61:$S$66</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Data!$T$61:$T$66</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Data!$S$61:$S$66</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Data!$T$61:$T$66</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="36">
   <si>
     <t>Attempt</t>
   </si>
@@ -121,6 +123,24 @@
   <si>
     <t>Sort on List of length 20000</t>
   </si>
+  <si>
+    <t>Duplicates on List of length 10</t>
+  </si>
+  <si>
+    <t>Duplicates on List of length 100</t>
+  </si>
+  <si>
+    <t>Duplicates on List of length 1000</t>
+  </si>
+  <si>
+    <t>Duplicates on List of length 5000</t>
+  </si>
+  <si>
+    <t>Duplicates on List of length 10000</t>
+  </si>
+  <si>
+    <t>Duplicates on List of length 20000</t>
+  </si>
 </sst>
 </file>
 
@@ -135,7 +155,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB4E3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -231,25 +257,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -259,12 +273,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -274,12 +282,40 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB4E3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1720,6 +1756,363 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Duplicates Method</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$S$61:$S$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$T$61:$T$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.3579999999999975E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7129999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7689999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11685999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15751999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15762999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E20-8348-9F67-F6ECA8C5B14F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1017411695"/>
+        <c:axId val="1017413375"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1017411695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1017413375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1017413375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1017411695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1880,6 +2273,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -3495,6 +3928,544 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4186,6 +5157,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90FBF4FF-A78C-2E44-A42F-F3528AD42F3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4486,2237 +5495,2782 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D4128A-2966-F54D-A276-45E672D85F83}">
-  <dimension ref="A1:T55"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
     <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" customWidth="1"/>
     <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" customWidth="1"/>
     <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="22"/>
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="22"/>
+      <c r="G1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="1" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="K1" s="22"/>
+      <c r="M1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="P1" s="1" t="s">
+      <c r="N1" s="22"/>
+      <c r="P1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="1"/>
+      <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="19">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>1</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="14">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>1</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <v>1</v>
       </c>
-      <c r="Q3" s="20">
+      <c r="Q3" s="14">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="S3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="18"/>
+      <c r="T3" s="21"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="19">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>2</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>2</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="14">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>2</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="1">
         <v>2</v>
       </c>
-      <c r="Q4" s="20">
+      <c r="Q4" s="14">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="S4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="12" t="s">
+      <c r="T4" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>1E-4</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>3</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>3</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="14">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <v>3</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <v>3</v>
       </c>
-      <c r="Q5" s="20">
+      <c r="Q5" s="14">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="S5" s="12">
+      <c r="S5" s="8">
         <v>10</v>
       </c>
-      <c r="T5" s="12">
+      <c r="T5" s="8">
         <f>B13</f>
         <v>4.5000000000000015E-4</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1E-4</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>4</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>1E-4</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>4</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>1E-4</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>4</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="14">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="1">
         <v>4</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="1">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="1">
         <v>4</v>
       </c>
-      <c r="Q6" s="20">
+      <c r="Q6" s="14">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="S6" s="12">
+      <c r="S6" s="8">
         <v>100</v>
       </c>
-      <c r="T6" s="12">
+      <c r="T6" s="8">
         <f>E13</f>
         <v>5.0000000000000023E-4</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>1E-4</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>5</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>5</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K7" s="14">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="1">
         <v>5</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="1">
         <v>5</v>
       </c>
-      <c r="Q7" s="20">
+      <c r="Q7" s="14">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="S7" s="12">
+      <c r="S7" s="8">
         <v>1000</v>
       </c>
-      <c r="T7" s="12">
+      <c r="T7" s="8">
         <f>H13</f>
         <v>5.2099999999999998E-4</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
+      <c r="A8" s="13">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>0</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>6</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>1E-4</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>6</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>1E-4</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <v>6</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="14">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="1">
         <v>6</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="1">
         <v>6</v>
       </c>
-      <c r="Q8" s="20">
+      <c r="Q8" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="S8" s="16">
+      <c r="S8" s="12">
         <v>5000</v>
       </c>
-      <c r="T8" s="16">
+      <c r="T8" s="12">
         <f>K13</f>
         <v>7.0999999999999991E-4</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="19">
+      <c r="A9" s="13">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>1E-4</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>7</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>1E-4</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>7</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>1E-4</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <v>7</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="1">
         <v>7</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="1">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="1">
         <v>7</v>
       </c>
-      <c r="Q9" s="20">
+      <c r="Q9" s="14">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="S9" s="12">
+      <c r="S9" s="8">
         <v>10000</v>
       </c>
-      <c r="T9" s="12">
+      <c r="T9" s="8">
         <f>N13</f>
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="19">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>8</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>1E-4</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>8</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
         <v>8</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="14">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="1">
         <v>8</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="1">
         <v>8</v>
       </c>
-      <c r="Q10" s="20">
+      <c r="Q10" s="14">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="S10" s="25">
+      <c r="S10" s="19">
         <v>20000</v>
       </c>
-      <c r="T10" s="12">
+      <c r="T10" s="8">
         <f>Q13</f>
         <v>1.1099999999999999E-3</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="19">
+      <c r="A11" s="13">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>1E-4</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>9</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>1E-4</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>9</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <v>9</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11" s="14">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="1">
         <v>9</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="1">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="1">
         <v>9</v>
       </c>
-      <c r="Q11" s="20">
+      <c r="Q11" s="14">
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="19">
+      <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>0</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>10</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>1E-4</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>10</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>1E-4</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>10</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="14">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="1">
         <v>10</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="1">
         <v>10</v>
       </c>
-      <c r="Q12" s="20">
+      <c r="Q12" s="14">
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <f>AVERAGE(B3:B12)</f>
         <v>4.5000000000000015E-4</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <f>AVERAGE(E3:E12)</f>
         <v>5.0000000000000023E-4</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <f>AVERAGE(H3:H12)</f>
         <v>5.2099999999999998E-4</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <f>AVERAGE(K3:K12)</f>
         <v>7.0999999999999991E-4</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="1">
         <f>AVERAGE(N3:N12)</f>
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="Q13" s="1">
         <f>AVERAGE(Q3:Q12)</f>
         <v>1.1099999999999999E-3</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="D15" s="3" t="s">
+      <c r="B15" s="23"/>
+      <c r="D15" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="G15" s="3" t="s">
+      <c r="E15" s="23"/>
+      <c r="G15" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="3" t="s">
+      <c r="H15" s="23"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="M15" s="3" t="s">
+      <c r="K15" s="23"/>
+      <c r="M15" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="3"/>
-      <c r="P15" s="3" t="s">
+      <c r="N15" s="23"/>
+      <c r="P15" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="Q15" s="3"/>
+      <c r="Q15" s="23"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="N16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P16" s="4" t="s">
+      <c r="P16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="Q16" s="4" t="s">
+      <c r="Q16" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="21">
+      <c r="A17" s="15">
         <v>1</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="2">
         <v>1.2E-2</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="2">
         <v>1</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="16">
         <v>1.01E-2</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="2">
         <v>1</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="3">
         <v>1.14E-2</v>
       </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="4">
+      <c r="I17" s="11"/>
+      <c r="J17" s="2">
         <v>1</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="3">
         <v>1.38E-2</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="2">
         <v>1</v>
       </c>
-      <c r="N17" s="22">
+      <c r="N17" s="16">
         <v>1.6E-2</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P17" s="2">
         <v>1</v>
       </c>
-      <c r="Q17" s="5">
+      <c r="Q17" s="3">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="S17" s="17" t="s">
+      <c r="S17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="T17" s="18"/>
+      <c r="T17" s="21"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="21">
+      <c r="A18" s="15">
         <v>2</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="2">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="2">
         <v>2</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="16">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="2">
         <v>2</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="3">
         <v>1E-3</v>
       </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="4">
+      <c r="I18" s="11"/>
+      <c r="J18" s="2">
         <v>2</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="3">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="2">
         <v>2</v>
       </c>
-      <c r="N18" s="22">
+      <c r="N18" s="16">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18" s="2">
         <v>2</v>
       </c>
-      <c r="Q18" s="5">
+      <c r="Q18" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="S18" s="12" t="s">
+      <c r="S18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="T18" s="12" t="s">
+      <c r="T18" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="21">
+      <c r="A19" s="15">
         <v>3</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="2">
         <v>1E-4</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="2">
         <v>3</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="16">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="2">
         <v>3</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="3">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="4">
+      <c r="I19" s="11"/>
+      <c r="J19" s="2">
         <v>3</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="3">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19" s="2">
         <v>3</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19" s="16">
         <v>4.1999999999999997E-3</v>
       </c>
-      <c r="P19" s="4">
+      <c r="P19" s="2">
         <v>3</v>
       </c>
-      <c r="Q19" s="5">
+      <c r="Q19" s="3">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="S19" s="12">
+      <c r="S19" s="8">
         <v>10</v>
       </c>
-      <c r="T19" s="12">
+      <c r="T19" s="8">
         <f>B27</f>
         <v>1.3499999999999996E-3</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="21">
+      <c r="A20" s="15">
         <v>4</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="2">
         <v>1E-4</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="2">
         <v>4</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="16">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="2">
         <v>4</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="3">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="4">
+      <c r="I20" s="11"/>
+      <c r="J20" s="2">
         <v>4</v>
       </c>
-      <c r="K20" s="5">
+      <c r="K20" s="3">
         <v>3.3E-3</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="2">
         <v>4</v>
       </c>
-      <c r="N20" s="22">
+      <c r="N20" s="16">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20" s="2">
         <v>4</v>
       </c>
-      <c r="Q20" s="5">
+      <c r="Q20" s="3">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="S20" s="12">
+      <c r="S20" s="8">
         <v>100</v>
       </c>
-      <c r="T20" s="12">
+      <c r="T20" s="8">
         <f>E27</f>
         <v>1.2100000000000004E-3</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="21">
+      <c r="A21" s="15">
         <v>5</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="2">
         <v>1E-4</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="2">
         <v>5</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="16">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="2">
         <v>5</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="3">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="4">
+      <c r="I21" s="11"/>
+      <c r="J21" s="2">
         <v>5</v>
       </c>
-      <c r="K21" s="5">
+      <c r="K21" s="3">
         <v>2.8E-3</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="2">
         <v>5</v>
       </c>
-      <c r="N21" s="22">
+      <c r="N21" s="16">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="P21" s="4">
+      <c r="P21" s="2">
         <v>5</v>
       </c>
-      <c r="Q21" s="5">
+      <c r="Q21" s="3">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="S21" s="12">
+      <c r="S21" s="8">
         <v>1000</v>
       </c>
-      <c r="T21" s="12">
+      <c r="T21" s="8">
         <f>H27</f>
         <v>1.83E-3</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="21">
+      <c r="A22" s="15">
         <v>6</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="2">
         <v>1E-4</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="2">
         <v>6</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="16">
         <v>1E-4</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="2">
         <v>6</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="3">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="4">
+      <c r="I22" s="11"/>
+      <c r="J22" s="2">
         <v>6</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22" s="3">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22" s="2">
         <v>6</v>
       </c>
-      <c r="N22" s="22">
+      <c r="N22" s="16">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="P22" s="4">
+      <c r="P22" s="2">
         <v>6</v>
       </c>
-      <c r="Q22" s="5">
+      <c r="Q22" s="3">
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="S22" s="16">
+      <c r="S22" s="12">
         <v>5000</v>
       </c>
-      <c r="T22" s="16">
+      <c r="T22" s="12">
         <f>K27</f>
         <v>3.919999999999999E-3</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A23" s="21">
+      <c r="A23" s="15">
         <v>7</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="2">
         <v>7</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="16">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="2">
         <v>7</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="3">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="4">
+      <c r="I23" s="11"/>
+      <c r="J23" s="2">
         <v>7</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23" s="3">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23" s="2">
         <v>7</v>
       </c>
-      <c r="N23" s="22">
+      <c r="N23" s="16">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="P23" s="4">
+      <c r="P23" s="2">
         <v>7</v>
       </c>
-      <c r="Q23" s="5">
+      <c r="Q23" s="3">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="S23" s="12">
+      <c r="S23" s="8">
         <v>10000</v>
       </c>
-      <c r="T23" s="12">
+      <c r="T23" s="8">
         <f>N27</f>
         <v>5.7499999999999999E-3</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24" s="21">
+      <c r="A24" s="15">
         <v>8</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="2">
         <v>1E-4</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="2">
         <v>8</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="16">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="2">
         <v>8</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="3">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="4">
+      <c r="I24" s="11"/>
+      <c r="J24" s="2">
         <v>8</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K24" s="3">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24" s="2">
         <v>8</v>
       </c>
-      <c r="N24" s="22">
+      <c r="N24" s="16">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="P24" s="4">
+      <c r="P24" s="2">
         <v>8</v>
       </c>
-      <c r="Q24" s="5">
+      <c r="Q24" s="3">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="S24" s="25">
+      <c r="S24" s="19">
         <v>20000</v>
       </c>
-      <c r="T24" s="12">
+      <c r="T24" s="8">
         <f>Q27</f>
         <v>1.0360000000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25" s="21">
+      <c r="A25" s="15">
         <v>9</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="2">
         <v>1E-4</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="2">
         <v>9</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="16">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="2">
         <v>9</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="3">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="4">
+      <c r="I25" s="11"/>
+      <c r="J25" s="2">
         <v>9</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K25" s="3">
         <v>2.8E-3</v>
       </c>
-      <c r="M25" s="4">
+      <c r="M25" s="2">
         <v>9</v>
       </c>
-      <c r="N25" s="22">
+      <c r="N25" s="16">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="P25" s="4">
+      <c r="P25" s="2">
         <v>9</v>
       </c>
-      <c r="Q25" s="5">
+      <c r="Q25" s="3">
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="21">
+      <c r="A26" s="15">
         <v>10</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="2">
         <v>1E-4</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="2">
         <v>10</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="16">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="2">
         <v>10</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="3">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="I26" s="15"/>
-      <c r="J26" s="4">
+      <c r="I26" s="11"/>
+      <c r="J26" s="2">
         <v>10</v>
       </c>
-      <c r="K26" s="5">
+      <c r="K26" s="3">
         <v>2.8E-3</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M26" s="2">
         <v>10</v>
       </c>
-      <c r="N26" s="22">
+      <c r="N26" s="16">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="P26" s="4">
+      <c r="P26" s="2">
         <v>10</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="Q26" s="3">
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="2">
         <f>AVERAGE(B17:B26)</f>
         <v>1.3499999999999996E-3</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="2">
         <f>AVERAGE(E17:E26)</f>
         <v>1.2100000000000004E-3</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="2">
         <f>AVERAGE(H17:H26)</f>
         <v>1.83E-3</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="2">
         <f>AVERAGE(K17:K26)</f>
         <v>3.919999999999999E-3</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="M27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N27" s="4">
+      <c r="N27" s="2">
         <f>AVERAGE(N17:N26)</f>
         <v>5.7499999999999999E-3</v>
       </c>
-      <c r="P27" s="4" t="s">
+      <c r="P27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q27" s="4">
+      <c r="Q27" s="2">
         <f>AVERAGE(Q17:Q26)</f>
         <v>1.0360000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="D29" s="6" t="s">
+      <c r="B29" s="24"/>
+      <c r="D29" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="G29" s="6" t="s">
+      <c r="E29" s="24"/>
+      <c r="G29" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="6"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="6" t="s">
+      <c r="H29" s="24"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="K29" s="6"/>
-      <c r="M29" s="6" t="s">
+      <c r="K29" s="24"/>
+      <c r="M29" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="N29" s="6"/>
-      <c r="P29" s="6" t="s">
+      <c r="N29" s="24"/>
+      <c r="P29" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="Q29" s="6"/>
+      <c r="Q29" s="24"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="7" t="s">
+      <c r="J30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K30" s="7" t="s">
+      <c r="K30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M30" s="7" t="s">
+      <c r="M30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="N30" s="7" t="s">
+      <c r="N30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P30" s="7" t="s">
+      <c r="P30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="Q30" s="7" t="s">
+      <c r="Q30" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="23">
+      <c r="A31" s="17">
         <v>1</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="5">
         <v>0.442</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="4">
         <v>1</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="5">
         <v>0.438</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="4">
         <v>1</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="5">
         <v>0.49809999999999999</v>
       </c>
-      <c r="I31" s="15"/>
-      <c r="J31" s="7">
+      <c r="I31" s="11"/>
+      <c r="J31" s="4">
         <v>1</v>
       </c>
-      <c r="K31" s="8">
+      <c r="K31" s="5">
         <v>0.98660000000000003</v>
       </c>
-      <c r="M31" s="7">
+      <c r="M31" s="4">
         <v>1</v>
       </c>
-      <c r="N31" s="8">
+      <c r="N31" s="5">
         <v>2.4782999999999999</v>
       </c>
-      <c r="P31" s="7">
+      <c r="P31" s="4">
         <v>1</v>
       </c>
-      <c r="Q31" s="8">
+      <c r="Q31" s="5">
         <v>10.633699999999999</v>
       </c>
-      <c r="S31" s="17" t="s">
+      <c r="S31" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="T31" s="18"/>
+      <c r="T31" s="21"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="23">
+      <c r="A32" s="17">
         <v>2</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="5">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="4">
         <v>2</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="5">
         <v>7.7999999999999996E-3</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="4">
         <v>2</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="5">
         <v>6.88E-2</v>
       </c>
-      <c r="I32" s="15"/>
-      <c r="J32" s="7">
+      <c r="I32" s="11"/>
+      <c r="J32" s="4">
         <v>2</v>
       </c>
-      <c r="K32" s="8">
+      <c r="K32" s="5">
         <v>0.52710000000000001</v>
       </c>
-      <c r="M32" s="7">
+      <c r="M32" s="4">
         <v>2</v>
       </c>
-      <c r="N32" s="8">
+      <c r="N32" s="5">
         <v>1.948</v>
       </c>
-      <c r="P32" s="7">
+      <c r="P32" s="4">
         <v>2</v>
       </c>
-      <c r="Q32" s="8">
+      <c r="Q32" s="5">
         <v>10.061299999999999</v>
       </c>
-      <c r="S32" s="12" t="s">
+      <c r="S32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="T32" s="12" t="s">
+      <c r="T32" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A33" s="23">
+      <c r="A33" s="17">
         <v>3</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="5">
         <v>7.7999999999999996E-3</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="4">
         <v>3</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="5">
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="4">
         <v>3</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="5">
         <v>6.0499999999999998E-2</v>
       </c>
-      <c r="I33" s="15"/>
-      <c r="J33" s="7">
+      <c r="I33" s="11"/>
+      <c r="J33" s="4">
         <v>3</v>
       </c>
-      <c r="K33" s="8">
+      <c r="K33" s="5">
         <v>0.56979999999999997</v>
       </c>
-      <c r="M33" s="7">
+      <c r="M33" s="4">
         <v>3</v>
       </c>
-      <c r="N33" s="8">
+      <c r="N33" s="5">
         <v>1.9652000000000001</v>
       </c>
-      <c r="P33" s="7">
+      <c r="P33" s="4">
         <v>3</v>
       </c>
-      <c r="Q33" s="8">
+      <c r="Q33" s="5">
         <v>10.1968</v>
       </c>
-      <c r="S33" s="12">
+      <c r="S33" s="8">
         <v>10</v>
       </c>
-      <c r="T33" s="12">
+      <c r="T33" s="8">
         <f>B41</f>
         <v>4.6909999999999993E-2</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A34" s="23">
+      <c r="A34" s="17">
         <v>4</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="5">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="4">
         <v>4</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="5">
         <v>6.6E-3</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="4">
         <v>4</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34" s="5">
         <v>8.7900000000000006E-2</v>
       </c>
-      <c r="I34" s="15"/>
-      <c r="J34" s="7">
+      <c r="I34" s="11"/>
+      <c r="J34" s="4">
         <v>4</v>
       </c>
-      <c r="K34" s="8">
+      <c r="K34" s="5">
         <v>0.53759999999999997</v>
       </c>
-      <c r="M34" s="7">
+      <c r="M34" s="4">
         <v>4</v>
       </c>
-      <c r="N34" s="8">
+      <c r="N34" s="5">
         <v>1.9508000000000001</v>
       </c>
-      <c r="P34" s="7">
+      <c r="P34" s="4">
         <v>4</v>
       </c>
-      <c r="Q34" s="8">
+      <c r="Q34" s="5">
         <v>10.1976</v>
       </c>
-      <c r="S34" s="12">
+      <c r="S34" s="8">
         <v>100</v>
       </c>
-      <c r="T34" s="12">
+      <c r="T34" s="8">
         <f>E41</f>
         <v>5.0169999999999992E-2</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A35" s="23">
+      <c r="A35" s="17">
         <v>5</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="5">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="4">
         <v>5</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="5">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="4">
         <v>5</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="5">
         <v>6.0600000000000001E-2</v>
       </c>
-      <c r="I35" s="15"/>
-      <c r="J35" s="7">
+      <c r="I35" s="11"/>
+      <c r="J35" s="4">
         <v>5</v>
       </c>
-      <c r="K35" s="8">
+      <c r="K35" s="5">
         <v>0.5302</v>
       </c>
-      <c r="M35" s="7">
+      <c r="M35" s="4">
         <v>5</v>
       </c>
-      <c r="N35" s="8">
+      <c r="N35" s="5">
         <v>2.1080000000000001</v>
       </c>
-      <c r="P35" s="7">
+      <c r="P35" s="4">
         <v>5</v>
       </c>
-      <c r="Q35" s="8">
+      <c r="Q35" s="5">
         <v>10.130599999999999</v>
       </c>
-      <c r="S35" s="12">
+      <c r="S35" s="8">
         <v>1000</v>
       </c>
-      <c r="T35" s="12">
+      <c r="T35" s="8">
         <f>H41</f>
         <v>0.10834999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A36" s="23">
+      <c r="A36" s="17">
         <v>6</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="5">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="4">
         <v>6</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="5">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="4">
         <v>6</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="5">
         <v>5.79E-2</v>
       </c>
-      <c r="I36" s="15"/>
-      <c r="J36" s="7">
+      <c r="I36" s="11"/>
+      <c r="J36" s="4">
         <v>6</v>
       </c>
-      <c r="K36" s="8">
+      <c r="K36" s="5">
         <v>0.52680000000000005</v>
       </c>
-      <c r="M36" s="7">
+      <c r="M36" s="4">
         <v>6</v>
       </c>
-      <c r="N36" s="8">
+      <c r="N36" s="5">
         <v>1.9117</v>
       </c>
-      <c r="P36" s="7">
+      <c r="P36" s="4">
         <v>6</v>
       </c>
-      <c r="Q36" s="8">
+      <c r="Q36" s="5">
         <v>9.8620000000000001</v>
       </c>
-      <c r="S36" s="16">
+      <c r="S36" s="12">
         <v>5000</v>
       </c>
-      <c r="T36" s="16">
+      <c r="T36" s="12">
         <f>K41</f>
         <v>0.63792000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="23">
+      <c r="A37" s="17">
         <v>7</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="5">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="4">
         <v>7</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="5">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="4">
         <v>7</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="5">
         <v>6.59E-2</v>
       </c>
-      <c r="I37" s="15"/>
-      <c r="J37" s="7">
+      <c r="I37" s="11"/>
+      <c r="J37" s="4">
         <v>7</v>
       </c>
-      <c r="K37" s="8">
+      <c r="K37" s="5">
         <v>1.0561</v>
       </c>
-      <c r="M37" s="7">
+      <c r="M37" s="4">
         <v>7</v>
       </c>
-      <c r="N37" s="8">
+      <c r="N37" s="5">
         <v>1.9253</v>
       </c>
-      <c r="P37" s="7">
+      <c r="P37" s="4">
         <v>7</v>
       </c>
-      <c r="Q37" s="8">
+      <c r="Q37" s="5">
         <v>9.5998000000000001</v>
       </c>
-      <c r="S37" s="12">
+      <c r="S37" s="8">
         <v>10000</v>
       </c>
-      <c r="T37" s="12">
+      <c r="T37" s="8">
         <f>N41</f>
         <v>2.0643500000000001</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A38" s="23">
+      <c r="A38" s="17">
         <v>8</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="5">
         <v>2.3E-3</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="4">
         <v>8</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="5">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="4">
         <v>8</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="5">
         <v>5.8400000000000001E-2</v>
       </c>
-      <c r="I38" s="15"/>
-      <c r="J38" s="7">
+      <c r="I38" s="11"/>
+      <c r="J38" s="4">
         <v>8</v>
       </c>
-      <c r="K38" s="8">
+      <c r="K38" s="5">
         <v>0.58199999999999996</v>
       </c>
-      <c r="M38" s="7">
+      <c r="M38" s="4">
         <v>8</v>
       </c>
-      <c r="N38" s="8">
+      <c r="N38" s="5">
         <v>1.9898</v>
       </c>
-      <c r="P38" s="7">
+      <c r="P38" s="4">
         <v>8</v>
       </c>
-      <c r="Q38" s="8">
+      <c r="Q38" s="5">
         <v>9.6417999999999999</v>
       </c>
-      <c r="S38" s="25">
+      <c r="S38" s="19">
         <v>20000</v>
       </c>
-      <c r="T38" s="12">
+      <c r="T38" s="8">
         <f>Q41</f>
         <v>10.04461</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A39" s="23">
+      <c r="A39" s="17">
         <v>9</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="5">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="4">
         <v>9</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="5">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="4">
         <v>9</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39" s="5">
         <v>5.8700000000000002E-2</v>
       </c>
-      <c r="I39" s="15"/>
-      <c r="J39" s="7">
+      <c r="I39" s="11"/>
+      <c r="J39" s="4">
         <v>9</v>
       </c>
-      <c r="K39" s="8">
+      <c r="K39" s="5">
         <v>0.51970000000000005</v>
       </c>
-      <c r="M39" s="7">
+      <c r="M39" s="4">
         <v>9</v>
       </c>
-      <c r="N39" s="8">
+      <c r="N39" s="5">
         <v>2.1677</v>
       </c>
-      <c r="P39" s="7">
+      <c r="P39" s="4">
         <v>9</v>
       </c>
-      <c r="Q39" s="8">
+      <c r="Q39" s="5">
         <v>9.8323999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A40" s="23">
+      <c r="A40" s="17">
         <v>10</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="5">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="4">
         <v>10</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="5">
         <v>7.1000000000000004E-3</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40" s="4">
         <v>10</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H40" s="5">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="I40" s="15"/>
-      <c r="J40" s="7">
+      <c r="I40" s="11"/>
+      <c r="J40" s="4">
         <v>10</v>
       </c>
-      <c r="K40" s="8">
+      <c r="K40" s="5">
         <v>0.54330000000000001</v>
       </c>
-      <c r="M40" s="7">
+      <c r="M40" s="4">
         <v>10</v>
       </c>
-      <c r="N40" s="8">
+      <c r="N40" s="5">
         <v>2.1987000000000001</v>
       </c>
-      <c r="P40" s="7">
+      <c r="P40" s="4">
         <v>10</v>
       </c>
-      <c r="Q40" s="8">
+      <c r="Q40" s="5">
         <v>10.290100000000001</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="4">
         <f>AVERAGE(B31:B40)</f>
         <v>4.6909999999999993E-2</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="4">
         <f>AVERAGE(E31:E40)</f>
         <v>5.0169999999999992E-2</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="4">
         <f>AVERAGE(H31:H40)</f>
         <v>0.10834999999999999</v>
       </c>
-      <c r="J41" s="7" t="s">
+      <c r="J41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K41" s="7">
+      <c r="K41" s="4">
         <f>AVERAGE(K31:K40)</f>
         <v>0.63792000000000004</v>
       </c>
-      <c r="M41" s="7" t="s">
+      <c r="M41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="7">
+      <c r="N41" s="4">
         <f>AVERAGE(N31:N40)</f>
         <v>2.0643500000000001</v>
       </c>
-      <c r="P41" s="7" t="s">
+      <c r="P41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q41" s="7">
+      <c r="Q41" s="4">
         <f>AVERAGE(Q31:Q40)</f>
         <v>10.04461</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="D43" s="9" t="s">
+      <c r="B43" s="25"/>
+      <c r="D43" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="9"/>
-      <c r="G43" s="9" t="s">
+      <c r="E43" s="25"/>
+      <c r="G43" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="H43" s="9"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="9" t="s">
+      <c r="H43" s="25"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K43" s="9"/>
-      <c r="M43" s="9" t="s">
+      <c r="K43" s="25"/>
+      <c r="M43" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="N43" s="9"/>
-      <c r="P43" s="9" t="s">
+      <c r="N43" s="25"/>
+      <c r="P43" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="Q43" s="9"/>
+      <c r="Q43" s="25"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="G44" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="H44" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J44" s="10" t="s">
+      <c r="J44" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="K44" s="10" t="s">
+      <c r="K44" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M44" s="10" t="s">
+      <c r="M44" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N44" s="10" t="s">
+      <c r="N44" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="P44" s="10" t="s">
+      <c r="P44" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="Q44" s="10" t="s">
+      <c r="Q44" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A45" s="24">
+      <c r="A45" s="18">
         <v>1</v>
       </c>
-      <c r="B45" s="11">
+      <c r="B45" s="7">
         <v>2.0199999999999999E-2</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="6">
         <v>1</v>
       </c>
-      <c r="E45" s="11">
+      <c r="E45" s="7">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="G45" s="10">
+      <c r="G45" s="6">
         <v>1</v>
       </c>
-      <c r="H45" s="11">
+      <c r="H45" s="7">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="I45" s="15"/>
-      <c r="J45" s="10">
+      <c r="I45" s="11"/>
+      <c r="J45" s="6">
         <v>1</v>
       </c>
-      <c r="K45" s="11">
+      <c r="K45" s="7">
         <v>0.1341</v>
       </c>
-      <c r="M45" s="10">
+      <c r="M45" s="6">
         <v>1</v>
       </c>
-      <c r="N45" s="11">
+      <c r="N45" s="7">
         <v>0.25779999999999997</v>
       </c>
-      <c r="P45" s="10">
+      <c r="P45" s="6">
         <v>1</v>
       </c>
-      <c r="Q45" s="11">
+      <c r="Q45" s="7">
         <v>0.48559999999999998</v>
       </c>
-      <c r="S45" s="17" t="s">
+      <c r="S45" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="T45" s="18"/>
+      <c r="T45" s="21"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A46" s="24">
+      <c r="A46" s="18">
         <v>2</v>
       </c>
-      <c r="B46" s="11">
+      <c r="B46" s="7">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="6">
         <v>2</v>
       </c>
-      <c r="E46" s="11">
+      <c r="E46" s="7">
         <v>2.8E-3</v>
       </c>
-      <c r="G46" s="10">
+      <c r="G46" s="6">
         <v>2</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H46" s="7">
         <v>2.23E-2</v>
       </c>
-      <c r="I46" s="15"/>
-      <c r="J46" s="10">
+      <c r="I46" s="11"/>
+      <c r="J46" s="6">
         <v>2</v>
       </c>
-      <c r="K46" s="11">
+      <c r="K46" s="7">
         <v>0.1174</v>
       </c>
-      <c r="M46" s="10">
+      <c r="M46" s="6">
         <v>2</v>
       </c>
-      <c r="N46" s="11">
+      <c r="N46" s="7">
         <v>0.34989999999999999</v>
       </c>
-      <c r="P46" s="10">
+      <c r="P46" s="6">
         <v>2</v>
       </c>
-      <c r="Q46" s="11">
+      <c r="Q46" s="7">
         <v>0.51990000000000003</v>
       </c>
-      <c r="S46" s="12" t="s">
+      <c r="S46" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="T46" s="12" t="s">
+      <c r="T46" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A47" s="24">
+      <c r="A47" s="18">
         <v>3</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47" s="7">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="6">
         <v>3</v>
       </c>
-      <c r="E47" s="11">
+      <c r="E47" s="7">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="G47" s="10">
+      <c r="G47" s="6">
         <v>3</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H47" s="7">
         <v>2.2200000000000001E-2</v>
       </c>
-      <c r="I47" s="15"/>
-      <c r="J47" s="10">
+      <c r="I47" s="11"/>
+      <c r="J47" s="6">
         <v>3</v>
       </c>
-      <c r="K47" s="11">
+      <c r="K47" s="7">
         <v>0.1089</v>
       </c>
-      <c r="M47" s="10">
+      <c r="M47" s="6">
         <v>3</v>
       </c>
-      <c r="N47" s="11">
+      <c r="N47" s="7">
         <v>0.2392</v>
       </c>
-      <c r="P47" s="10">
+      <c r="P47" s="6">
         <v>3</v>
       </c>
-      <c r="Q47" s="11">
+      <c r="Q47" s="7">
         <v>0.47360000000000002</v>
       </c>
-      <c r="S47" s="12">
+      <c r="S47" s="8">
         <v>10</v>
       </c>
-      <c r="T47" s="12">
+      <c r="T47" s="8">
         <f>B55</f>
         <v>2.2599999999999994E-3</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A48" s="24">
+      <c r="A48" s="18">
         <v>4</v>
       </c>
-      <c r="B48" s="11">
+      <c r="B48" s="7">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="6">
         <v>4</v>
       </c>
-      <c r="E48" s="11">
+      <c r="E48" s="7">
         <v>2.3E-3</v>
       </c>
-      <c r="G48" s="10">
+      <c r="G48" s="6">
         <v>4</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H48" s="7">
         <v>3.44E-2</v>
       </c>
-      <c r="I48" s="15"/>
-      <c r="J48" s="10">
+      <c r="I48" s="11"/>
+      <c r="J48" s="6">
         <v>4</v>
       </c>
-      <c r="K48" s="11">
+      <c r="K48" s="7">
         <v>0.1045</v>
       </c>
-      <c r="M48" s="10">
+      <c r="M48" s="6">
         <v>4</v>
       </c>
-      <c r="N48" s="11">
+      <c r="N48" s="7">
         <v>0.22889999999999999</v>
       </c>
-      <c r="P48" s="10">
+      <c r="P48" s="6">
         <v>4</v>
       </c>
-      <c r="Q48" s="11">
+      <c r="Q48" s="7">
         <v>0.48749999999999999</v>
       </c>
-      <c r="S48" s="12">
+      <c r="S48" s="8">
         <v>100</v>
       </c>
-      <c r="T48" s="12">
+      <c r="T48" s="8">
         <f>E55</f>
         <v>4.28E-3</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A49" s="24">
+      <c r="A49" s="18">
         <v>5</v>
       </c>
-      <c r="B49" s="11">
+      <c r="B49" s="7">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D49" s="6">
         <v>5</v>
       </c>
-      <c r="E49" s="11">
+      <c r="E49" s="7">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G49" s="10">
+      <c r="G49" s="6">
         <v>5</v>
       </c>
-      <c r="H49" s="11">
+      <c r="H49" s="7">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="I49" s="15"/>
-      <c r="J49" s="10">
+      <c r="I49" s="11"/>
+      <c r="J49" s="6">
         <v>5</v>
       </c>
-      <c r="K49" s="11">
+      <c r="K49" s="7">
         <v>0.1099</v>
       </c>
-      <c r="M49" s="10">
+      <c r="M49" s="6">
         <v>5</v>
       </c>
-      <c r="N49" s="11">
+      <c r="N49" s="7">
         <v>0.23619999999999999</v>
       </c>
-      <c r="P49" s="10">
+      <c r="P49" s="6">
         <v>5</v>
       </c>
-      <c r="Q49" s="11">
+      <c r="Q49" s="7">
         <v>0.46100000000000002</v>
       </c>
-      <c r="S49" s="12">
+      <c r="S49" s="8">
         <v>1000</v>
       </c>
-      <c r="T49" s="12">
+      <c r="T49" s="8">
         <f>H55</f>
         <v>2.5530000000000004E-2</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A50" s="24">
+      <c r="A50" s="18">
         <v>6</v>
       </c>
-      <c r="B50" s="11">
+      <c r="B50" s="7">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="6">
         <v>6</v>
       </c>
-      <c r="E50" s="11">
+      <c r="E50" s="7">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G50" s="10">
+      <c r="G50" s="6">
         <v>6</v>
       </c>
-      <c r="H50" s="11">
+      <c r="H50" s="7">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="I50" s="15"/>
-      <c r="J50" s="10">
+      <c r="I50" s="11"/>
+      <c r="J50" s="6">
         <v>6</v>
       </c>
-      <c r="K50" s="11">
+      <c r="K50" s="7">
         <v>0.10929999999999999</v>
       </c>
-      <c r="M50" s="10">
+      <c r="M50" s="6">
         <v>6</v>
       </c>
-      <c r="N50" s="11">
+      <c r="N50" s="7">
         <v>0.23</v>
       </c>
-      <c r="P50" s="10">
+      <c r="P50" s="6">
         <v>6</v>
       </c>
-      <c r="Q50" s="11">
+      <c r="Q50" s="7">
         <v>0.46760000000000002</v>
       </c>
-      <c r="S50" s="16">
+      <c r="S50" s="12">
         <v>5000</v>
       </c>
-      <c r="T50" s="16">
+      <c r="T50" s="12">
         <f>K55</f>
         <v>0.11646999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A51" s="24">
+      <c r="A51" s="18">
         <v>7</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="7">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D51" s="6">
         <v>7</v>
       </c>
-      <c r="E51" s="11">
+      <c r="E51" s="7">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="G51" s="10">
+      <c r="G51" s="6">
         <v>7</v>
       </c>
-      <c r="H51" s="11">
+      <c r="H51" s="7">
         <v>2.24E-2</v>
       </c>
-      <c r="I51" s="15"/>
-      <c r="J51" s="10">
+      <c r="I51" s="11"/>
+      <c r="J51" s="6">
         <v>7</v>
       </c>
-      <c r="K51" s="11">
+      <c r="K51" s="7">
         <v>0.1081</v>
       </c>
-      <c r="M51" s="10">
+      <c r="M51" s="6">
         <v>7</v>
       </c>
-      <c r="N51" s="11">
+      <c r="N51" s="7">
         <v>0.26250000000000001</v>
       </c>
-      <c r="P51" s="10">
+      <c r="P51" s="6">
         <v>7</v>
       </c>
-      <c r="Q51" s="11">
+      <c r="Q51" s="7">
         <v>0.45500000000000002</v>
       </c>
-      <c r="S51" s="12">
+      <c r="S51" s="8">
         <v>10000</v>
       </c>
-      <c r="T51" s="12">
+      <c r="T51" s="8">
         <f>N55</f>
         <v>0.25334000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A52" s="24">
+      <c r="A52" s="18">
         <v>8</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52" s="7">
         <v>1E-4</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="6">
         <v>8</v>
       </c>
-      <c r="E52" s="11">
+      <c r="E52" s="7">
         <v>2.3E-3</v>
       </c>
-      <c r="G52" s="10">
+      <c r="G52" s="6">
         <v>8</v>
       </c>
-      <c r="H52" s="11">
+      <c r="H52" s="7">
         <v>2.23E-2</v>
       </c>
-      <c r="I52" s="15"/>
-      <c r="J52" s="10">
+      <c r="I52" s="11"/>
+      <c r="J52" s="6">
         <v>8</v>
       </c>
-      <c r="K52" s="11">
+      <c r="K52" s="7">
         <v>0.1086</v>
       </c>
-      <c r="M52" s="10">
+      <c r="M52" s="6">
         <v>8</v>
       </c>
-      <c r="N52" s="11">
+      <c r="N52" s="7">
         <v>0.24529999999999999</v>
       </c>
-      <c r="P52" s="10">
+      <c r="P52" s="6">
         <v>8</v>
       </c>
-      <c r="Q52" s="11">
+      <c r="Q52" s="7">
         <v>0.46250000000000002</v>
       </c>
-      <c r="S52" s="12">
+      <c r="S52" s="8">
         <v>20000</v>
       </c>
-      <c r="T52" s="12">
+      <c r="T52" s="8">
         <f>Q55</f>
         <v>0.48839999999999995</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A53" s="24">
+      <c r="A53" s="18">
         <v>9</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="7">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D53" s="6">
         <v>9</v>
       </c>
-      <c r="E53" s="11">
+      <c r="E53" s="7">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="G53" s="10">
+      <c r="G53" s="6">
         <v>9</v>
       </c>
-      <c r="H53" s="11">
+      <c r="H53" s="7">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="I53" s="15"/>
-      <c r="J53" s="10">
+      <c r="I53" s="11"/>
+      <c r="J53" s="6">
         <v>9</v>
       </c>
-      <c r="K53" s="11">
+      <c r="K53" s="7">
         <v>0.15479999999999999</v>
       </c>
-      <c r="M53" s="10">
+      <c r="M53" s="6">
         <v>9</v>
       </c>
-      <c r="N53" s="11">
+      <c r="N53" s="7">
         <v>0.2525</v>
       </c>
-      <c r="P53" s="10">
+      <c r="P53" s="6">
         <v>9</v>
       </c>
-      <c r="Q53" s="11">
+      <c r="Q53" s="7">
         <v>0.59330000000000005</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A54" s="24">
+      <c r="A54" s="18">
         <v>10</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54" s="7">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D54" s="6">
         <v>10</v>
       </c>
-      <c r="E54" s="11">
+      <c r="E54" s="7">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="G54" s="10">
+      <c r="G54" s="6">
         <v>10</v>
       </c>
-      <c r="H54" s="11">
+      <c r="H54" s="7">
         <v>2.1899999999999999E-2</v>
       </c>
-      <c r="I54" s="15"/>
-      <c r="J54" s="10">
+      <c r="I54" s="11"/>
+      <c r="J54" s="6">
         <v>10</v>
       </c>
-      <c r="K54" s="11">
+      <c r="K54" s="7">
         <v>0.1091</v>
       </c>
-      <c r="M54" s="10">
+      <c r="M54" s="6">
         <v>10</v>
       </c>
-      <c r="N54" s="11">
+      <c r="N54" s="7">
         <v>0.2311</v>
       </c>
-      <c r="P54" s="10">
+      <c r="P54" s="6">
         <v>10</v>
       </c>
-      <c r="Q54" s="11">
+      <c r="Q54" s="7">
         <v>0.47799999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="10">
+      <c r="B55" s="6">
         <f>AVERAGE(B45:B54)</f>
         <v>2.2599999999999994E-3</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E55" s="10">
+      <c r="E55" s="6">
         <f>AVERAGE(E45:E54)</f>
         <v>4.28E-3</v>
       </c>
-      <c r="G55" s="10" t="s">
+      <c r="G55" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H55" s="10">
+      <c r="H55" s="6">
         <f>AVERAGE(H45:H54)</f>
         <v>2.5530000000000004E-2</v>
       </c>
-      <c r="J55" s="10" t="s">
+      <c r="J55" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K55" s="10">
+      <c r="K55" s="6">
         <f>AVERAGE(K45:K54)</f>
         <v>0.11646999999999999</v>
       </c>
-      <c r="M55" s="10" t="s">
+      <c r="M55" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="N55" s="10">
+      <c r="N55" s="6">
         <f>AVERAGE(N45:N54)</f>
         <v>0.25334000000000001</v>
       </c>
-      <c r="P55" s="10" t="s">
+      <c r="P55" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="Q55" s="10">
+      <c r="Q55" s="6">
         <f>AVERAGE(Q45:Q54)</f>
         <v>0.48839999999999995</v>
       </c>
     </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A57" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" s="26"/>
+      <c r="D57" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E57" s="26"/>
+      <c r="G57" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H57" s="26"/>
+      <c r="J57" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K57" s="26"/>
+      <c r="M57" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="N57" s="26"/>
+      <c r="P57" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q57" s="26"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A58" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G58" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="H58" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J58" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="K58" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="M58" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="N58" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="P58" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A59" s="27">
+        <v>1</v>
+      </c>
+      <c r="B59" s="28">
+        <v>0.52969999999999995</v>
+      </c>
+      <c r="D59" s="27">
+        <v>1</v>
+      </c>
+      <c r="E59" s="28">
+        <v>0.51219999999999999</v>
+      </c>
+      <c r="G59" s="27">
+        <v>1</v>
+      </c>
+      <c r="H59" s="28">
+        <v>0.62749999999999995</v>
+      </c>
+      <c r="J59" s="27">
+        <v>1</v>
+      </c>
+      <c r="K59" s="28">
+        <v>0.62160000000000004</v>
+      </c>
+      <c r="M59" s="27">
+        <v>1</v>
+      </c>
+      <c r="N59" s="28">
+        <v>0.75660000000000005</v>
+      </c>
+      <c r="P59" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="28">
+        <v>0.66080000000000005</v>
+      </c>
+      <c r="S59" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="T59" s="21"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A60" s="27">
+        <v>2</v>
+      </c>
+      <c r="B60" s="28">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="D60" s="27">
+        <v>2</v>
+      </c>
+      <c r="E60" s="28">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="G60" s="27">
+        <v>2</v>
+      </c>
+      <c r="H60" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="J60" s="27">
+        <v>2</v>
+      </c>
+      <c r="K60" s="28">
+        <v>2.46E-2</v>
+      </c>
+      <c r="M60" s="27">
+        <v>2</v>
+      </c>
+      <c r="N60" s="28">
+        <v>0.31069999999999998</v>
+      </c>
+      <c r="P60" s="27">
+        <v>2</v>
+      </c>
+      <c r="Q60" s="28">
+        <v>0.22850000000000001</v>
+      </c>
+      <c r="S60" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T60" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A61" s="27">
+        <v>3</v>
+      </c>
+      <c r="B61" s="28">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="D61" s="27">
+        <v>3</v>
+      </c>
+      <c r="E61" s="28">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="G61" s="27">
+        <v>3</v>
+      </c>
+      <c r="H61" s="28">
+        <v>3.3E-3</v>
+      </c>
+      <c r="J61" s="27">
+        <v>3</v>
+      </c>
+      <c r="K61" s="28">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="M61" s="27">
+        <v>3</v>
+      </c>
+      <c r="N61" s="28">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="P61" s="27">
+        <v>3</v>
+      </c>
+      <c r="Q61" s="28">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="S61" s="8">
+        <v>10</v>
+      </c>
+      <c r="T61" s="8">
+        <f>B69</f>
+        <v>5.3579999999999975E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62" s="27">
+        <v>4</v>
+      </c>
+      <c r="B62" s="28">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="D62" s="27">
+        <v>4</v>
+      </c>
+      <c r="E62" s="28">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="G62" s="27">
+        <v>4</v>
+      </c>
+      <c r="H62" s="28">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J62" s="27">
+        <v>4</v>
+      </c>
+      <c r="K62" s="28">
+        <v>5.67E-2</v>
+      </c>
+      <c r="M62" s="27">
+        <v>4</v>
+      </c>
+      <c r="N62" s="28">
+        <v>0.1132</v>
+      </c>
+      <c r="P62" s="27">
+        <v>4</v>
+      </c>
+      <c r="Q62" s="28">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="S62" s="8">
+        <v>100</v>
+      </c>
+      <c r="T62" s="8">
+        <f>E69</f>
+        <v>5.7129999999999993E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A63" s="27">
+        <v>5</v>
+      </c>
+      <c r="B63" s="28">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D63" s="27">
+        <v>5</v>
+      </c>
+      <c r="E63" s="28">
+        <v>1.06E-2</v>
+      </c>
+      <c r="G63" s="27">
+        <v>5</v>
+      </c>
+      <c r="H63" s="28">
+        <v>2.58E-2</v>
+      </c>
+      <c r="J63" s="27">
+        <v>5</v>
+      </c>
+      <c r="K63" s="28">
+        <v>5.7799999999999997E-2</v>
+      </c>
+      <c r="M63" s="27">
+        <v>5</v>
+      </c>
+      <c r="N63" s="28">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="P63" s="27">
+        <v>5</v>
+      </c>
+      <c r="Q63" s="28">
+        <v>0.2072</v>
+      </c>
+      <c r="S63" s="8">
+        <v>1000</v>
+      </c>
+      <c r="T63" s="8">
+        <f>H69</f>
+        <v>9.7689999999999999E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A64" s="27">
+        <v>6</v>
+      </c>
+      <c r="B64" s="28">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D64" s="27">
+        <v>6</v>
+      </c>
+      <c r="E64" s="28">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="G64" s="27">
+        <v>6</v>
+      </c>
+      <c r="H64" s="28">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J64" s="27">
+        <v>6</v>
+      </c>
+      <c r="K64" s="28">
+        <v>0.1114</v>
+      </c>
+      <c r="M64" s="27">
+        <v>6</v>
+      </c>
+      <c r="N64" s="28">
+        <v>3.9100000000000003E-2</v>
+      </c>
+      <c r="P64" s="27">
+        <v>6</v>
+      </c>
+      <c r="Q64" s="28">
+        <v>0.10580000000000001</v>
+      </c>
+      <c r="S64" s="12">
+        <v>5000</v>
+      </c>
+      <c r="T64" s="12">
+        <f>K69</f>
+        <v>0.11685999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A65" s="27">
+        <v>7</v>
+      </c>
+      <c r="B65" s="28">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D65" s="27">
+        <v>7</v>
+      </c>
+      <c r="E65" s="28">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="G65" s="27">
+        <v>7</v>
+      </c>
+      <c r="H65" s="28">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="J65" s="27">
+        <v>7</v>
+      </c>
+      <c r="K65" s="28">
+        <v>1.23E-2</v>
+      </c>
+      <c r="M65" s="27">
+        <v>7</v>
+      </c>
+      <c r="N65" s="28">
+        <v>2.64E-2</v>
+      </c>
+      <c r="P65" s="27">
+        <v>7</v>
+      </c>
+      <c r="Q65" s="28">
+        <v>6.0699999999999997E-2</v>
+      </c>
+      <c r="S65" s="8">
+        <v>10000</v>
+      </c>
+      <c r="T65" s="8">
+        <f>N69</f>
+        <v>0.15751999999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A66" s="27">
+        <v>8</v>
+      </c>
+      <c r="B66" s="28">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D66" s="27">
+        <v>8</v>
+      </c>
+      <c r="E66" s="28">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="G66" s="27">
+        <v>8</v>
+      </c>
+      <c r="H66" s="28">
+        <v>5.6099999999999997E-2</v>
+      </c>
+      <c r="J66" s="27">
+        <v>8</v>
+      </c>
+      <c r="K66" s="28">
+        <v>6.2799999999999995E-2</v>
+      </c>
+      <c r="M66" s="27">
+        <v>8</v>
+      </c>
+      <c r="N66" s="28">
+        <v>7.1499999999999994E-2</v>
+      </c>
+      <c r="P66" s="27">
+        <v>8</v>
+      </c>
+      <c r="Q66" s="28">
+        <v>0.13139999999999999</v>
+      </c>
+      <c r="S66" s="8">
+        <v>20000</v>
+      </c>
+      <c r="T66" s="8">
+        <f>Q69</f>
+        <v>0.15762999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A67" s="27">
+        <v>9</v>
+      </c>
+      <c r="B67" s="28">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D67" s="27">
+        <v>9</v>
+      </c>
+      <c r="E67" s="28">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="G67" s="27">
+        <v>9</v>
+      </c>
+      <c r="H67" s="28">
+        <v>8.5400000000000004E-2</v>
+      </c>
+      <c r="J67" s="27">
+        <v>9</v>
+      </c>
+      <c r="K67" s="28">
+        <v>0.1295</v>
+      </c>
+      <c r="M67" s="27">
+        <v>9</v>
+      </c>
+      <c r="N67" s="28">
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="P67" s="27">
+        <v>9</v>
+      </c>
+      <c r="Q67" s="28">
+        <v>1.5100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A68" s="27">
+        <v>10</v>
+      </c>
+      <c r="B68" s="28">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D68" s="27">
+        <v>10</v>
+      </c>
+      <c r="E68" s="28">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="G68" s="27">
+        <v>10</v>
+      </c>
+      <c r="H68" s="28">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="J68" s="27">
+        <v>10</v>
+      </c>
+      <c r="K68" s="28">
+        <v>7.0400000000000004E-2</v>
+      </c>
+      <c r="M68" s="27">
+        <v>10</v>
+      </c>
+      <c r="N68" s="28">
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="P68" s="27">
+        <v>10</v>
+      </c>
+      <c r="Q68" s="28">
+        <v>5.7599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A69" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="27">
+        <f>AVERAGE(B59:B68)</f>
+        <v>5.3579999999999975E-2</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" s="27">
+        <f>AVERAGE(E59:E68)</f>
+        <v>5.7129999999999993E-2</v>
+      </c>
+      <c r="G69" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H69" s="27">
+        <f>AVERAGE(H59:H68)</f>
+        <v>9.7689999999999999E-2</v>
+      </c>
+      <c r="J69" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K69" s="27">
+        <f>AVERAGE(K59:K68)</f>
+        <v>0.11685999999999999</v>
+      </c>
+      <c r="M69" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="N69" s="27">
+        <f>AVERAGE(N59:N68)</f>
+        <v>0.15751999999999997</v>
+      </c>
+      <c r="P69" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="27">
+        <f>AVERAGE(Q59:Q68)</f>
+        <v>0.15762999999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J43:K43"/>
+  <mergeCells count="35">
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="S59:T59"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="M15:N15"/>
     <mergeCell ref="S45:T45"/>
     <mergeCell ref="S31:T31"/>
     <mergeCell ref="A43:B43"/>
@@ -6727,14 +8281,16 @@
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="M29:N29"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P29:Q29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6745,7 +8301,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added timings for own Reverse method
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissasedgwick/Projects/Makers/Week_10/algorithmic_complexity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissasedgwick/Projects/Makers/Week_10/algorithmic-complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC7D9EE-60B9-D749-B916-131FFCEEBCE6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2839EA5-86F8-E74C-90D5-2A3A1784C5D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38420" yWindow="-10500" windowWidth="38400" windowHeight="21140" xr2:uid="{0EC00D74-CF7F-6E46-A448-9AC86E039AD3}"/>
+    <workbookView xWindow="-38400" yWindow="-10500" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{0EC00D74-CF7F-6E46-A448-9AC86E039AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Graphs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.2" hidden="1">Data!$S$61:$S$66</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Data!$T$61:$T$66</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Data!$S$61:$S$66</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Data!$T$61:$T$66</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Data!$S$75:$S$80</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Data!$T$75:$T$80</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Data!$S$75:$S$80</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Data!$T$75:$T$80</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="42">
   <si>
     <t>Attempt</t>
   </si>
@@ -141,6 +141,24 @@
   <si>
     <t>Duplicates on List of length 20000</t>
   </si>
+  <si>
+    <t>Own Reverse on List of length 100</t>
+  </si>
+  <si>
+    <t>Own Reverse on List of length 10</t>
+  </si>
+  <si>
+    <t>Own Reverse on List of length 1000</t>
+  </si>
+  <si>
+    <t>Own Reverse on List of length 5000</t>
+  </si>
+  <si>
+    <t>Own Reverse on List of length 10000</t>
+  </si>
+  <si>
+    <t>Own Reverse on List of length 20000</t>
+  </si>
 </sst>
 </file>
 
@@ -155,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +207,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFB4E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBE77FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -282,6 +306,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -294,17 +323,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -313,6 +342,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBE77FF"/>
       <color rgb="FFFFB4E3"/>
     </mruColors>
   </colors>
@@ -2113,6 +2143,367 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Reverse</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Own Method</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$S$75:$S$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$T$75:$T$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.3590000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.396E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.155E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1149999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1760000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9099999999999994E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7F28-FD48-9758-D3FE079D80B1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1664790736"/>
+        <c:axId val="1664792416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1664790736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1664792416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1664792416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1664790736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2313,6 +2704,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -4466,6 +4897,544 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5195,6 +6164,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F81271B-1908-394C-A421-3D84E9C92BFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5495,57 +6502,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D4128A-2966-F54D-A276-45E672D85F83}">
-  <dimension ref="A1:T69"/>
+  <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="T80" sqref="S75:T80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" style="10" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
     <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" customWidth="1"/>
     <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" customWidth="1"/>
-    <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.1640625" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" customWidth="1"/>
     <col min="19" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="25"/>
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="E1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="9"/>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="M1" s="22" t="s">
+      <c r="K1" s="25"/>
+      <c r="M1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="P1" s="22" t="s">
+      <c r="N1" s="25"/>
+      <c r="P1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="22"/>
+      <c r="Q1" s="25"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -5622,10 +6629,10 @@
       <c r="Q3" s="14">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="S3" s="20" t="s">
+      <c r="S3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="21"/>
+      <c r="T3" s="24"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
@@ -6062,31 +7069,31 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="D15" s="23" t="s">
+      <c r="B15" s="26"/>
+      <c r="D15" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="23"/>
-      <c r="G15" s="23" t="s">
+      <c r="E15" s="26"/>
+      <c r="G15" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="23"/>
+      <c r="H15" s="26"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="23"/>
-      <c r="M15" s="23" t="s">
+      <c r="K15" s="26"/>
+      <c r="M15" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="23"/>
-      <c r="P15" s="23" t="s">
+      <c r="N15" s="26"/>
+      <c r="P15" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="Q15" s="23"/>
+      <c r="Q15" s="26"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -6164,10 +7171,10 @@
       <c r="Q17" s="3">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="S17" s="20" t="s">
+      <c r="S17" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="T17" s="21"/>
+      <c r="T17" s="24"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
@@ -6613,31 +7620,31 @@
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="D29" s="24" t="s">
+      <c r="B29" s="28"/>
+      <c r="D29" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="24"/>
-      <c r="G29" s="24" t="s">
+      <c r="E29" s="28"/>
+      <c r="G29" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="24"/>
+      <c r="H29" s="28"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="24" t="s">
+      <c r="J29" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="K29" s="24"/>
-      <c r="M29" s="24" t="s">
+      <c r="K29" s="28"/>
+      <c r="M29" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="N29" s="24"/>
-      <c r="P29" s="24" t="s">
+      <c r="N29" s="28"/>
+      <c r="P29" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="Q29" s="24"/>
+      <c r="Q29" s="28"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
@@ -6715,10 +7722,10 @@
       <c r="Q31" s="5">
         <v>10.633699999999999</v>
       </c>
-      <c r="S31" s="20" t="s">
+      <c r="S31" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="T31" s="21"/>
+      <c r="T31" s="24"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="17">
@@ -7164,31 +8171,31 @@
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="D43" s="25" t="s">
+      <c r="B43" s="27"/>
+      <c r="D43" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="25"/>
-      <c r="G43" s="25" t="s">
+      <c r="E43" s="27"/>
+      <c r="G43" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="H43" s="25"/>
+      <c r="H43" s="27"/>
       <c r="I43" s="9"/>
-      <c r="J43" s="25" t="s">
+      <c r="J43" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K43" s="25"/>
-      <c r="M43" s="25" t="s">
+      <c r="K43" s="27"/>
+      <c r="M43" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="N43" s="25"/>
-      <c r="P43" s="25" t="s">
+      <c r="N43" s="27"/>
+      <c r="P43" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="Q43" s="25"/>
+      <c r="Q43" s="27"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
@@ -7266,10 +8273,10 @@
       <c r="Q45" s="7">
         <v>0.48559999999999998</v>
       </c>
-      <c r="S45" s="20" t="s">
+      <c r="S45" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="T45" s="21"/>
+      <c r="T45" s="24"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
@@ -7715,146 +8722,146 @@
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="26"/>
-      <c r="D57" s="26" t="s">
+      <c r="B57" s="22"/>
+      <c r="D57" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E57" s="26"/>
-      <c r="G57" s="26" t="s">
+      <c r="E57" s="22"/>
+      <c r="G57" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H57" s="26"/>
-      <c r="J57" s="26" t="s">
+      <c r="H57" s="22"/>
+      <c r="J57" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="K57" s="26"/>
-      <c r="M57" s="26" t="s">
+      <c r="K57" s="22"/>
+      <c r="M57" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="N57" s="26"/>
-      <c r="P57" s="26" t="s">
+      <c r="N57" s="22"/>
+      <c r="P57" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="Q57" s="26"/>
+      <c r="Q57" s="22"/>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A58" s="27" t="s">
+      <c r="A58" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="27" t="s">
+      <c r="D58" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E58" s="27" t="s">
+      <c r="E58" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="27" t="s">
+      <c r="G58" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H58" s="27" t="s">
+      <c r="H58" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J58" s="27" t="s">
+      <c r="J58" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K58" s="27" t="s">
+      <c r="K58" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="M58" s="27" t="s">
+      <c r="M58" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="N58" s="27" t="s">
+      <c r="N58" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="P58" s="27" t="s">
+      <c r="P58" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="Q58" s="27" t="s">
+      <c r="Q58" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A59" s="27">
+      <c r="A59" s="20">
         <v>1</v>
       </c>
-      <c r="B59" s="28">
+      <c r="B59" s="21">
         <v>0.52969999999999995</v>
       </c>
-      <c r="D59" s="27">
+      <c r="D59" s="20">
         <v>1</v>
       </c>
-      <c r="E59" s="28">
+      <c r="E59" s="21">
         <v>0.51219999999999999</v>
       </c>
-      <c r="G59" s="27">
+      <c r="G59" s="20">
         <v>1</v>
       </c>
-      <c r="H59" s="28">
+      <c r="H59" s="21">
         <v>0.62749999999999995</v>
       </c>
-      <c r="J59" s="27">
+      <c r="J59" s="20">
         <v>1</v>
       </c>
-      <c r="K59" s="28">
+      <c r="K59" s="21">
         <v>0.62160000000000004</v>
       </c>
-      <c r="M59" s="27">
+      <c r="M59" s="20">
         <v>1</v>
       </c>
-      <c r="N59" s="28">
+      <c r="N59" s="21">
         <v>0.75660000000000005</v>
       </c>
-      <c r="P59" s="27">
+      <c r="P59" s="20">
         <v>1</v>
       </c>
-      <c r="Q59" s="28">
+      <c r="Q59" s="21">
         <v>0.66080000000000005</v>
       </c>
-      <c r="S59" s="20" t="s">
+      <c r="S59" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="T59" s="21"/>
+      <c r="T59" s="24"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A60" s="27">
+      <c r="A60" s="20">
         <v>2</v>
       </c>
-      <c r="B60" s="28">
+      <c r="B60" s="21">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="D60" s="27">
+      <c r="D60" s="20">
         <v>2</v>
       </c>
-      <c r="E60" s="28">
+      <c r="E60" s="21">
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="G60" s="27">
+      <c r="G60" s="20">
         <v>2</v>
       </c>
-      <c r="H60" s="28">
+      <c r="H60" s="21">
         <v>0.02</v>
       </c>
-      <c r="J60" s="27">
+      <c r="J60" s="20">
         <v>2</v>
       </c>
-      <c r="K60" s="28">
+      <c r="K60" s="21">
         <v>2.46E-2</v>
       </c>
-      <c r="M60" s="27">
+      <c r="M60" s="20">
         <v>2</v>
       </c>
-      <c r="N60" s="28">
+      <c r="N60" s="21">
         <v>0.31069999999999998</v>
       </c>
-      <c r="P60" s="27">
+      <c r="P60" s="20">
         <v>2</v>
       </c>
-      <c r="Q60" s="28">
+      <c r="Q60" s="21">
         <v>0.22850000000000001</v>
       </c>
       <c r="S60" s="8" t="s">
@@ -7865,40 +8872,40 @@
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A61" s="27">
+      <c r="A61" s="20">
         <v>3</v>
       </c>
-      <c r="B61" s="28">
+      <c r="B61" s="21">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D61" s="27">
+      <c r="D61" s="20">
         <v>3</v>
       </c>
-      <c r="E61" s="28">
+      <c r="E61" s="21">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="G61" s="27">
+      <c r="G61" s="20">
         <v>3</v>
       </c>
-      <c r="H61" s="28">
+      <c r="H61" s="21">
         <v>3.3E-3</v>
       </c>
-      <c r="J61" s="27">
+      <c r="J61" s="20">
         <v>3</v>
       </c>
-      <c r="K61" s="28">
+      <c r="K61" s="21">
         <v>2.1499999999999998E-2</v>
       </c>
-      <c r="M61" s="27">
+      <c r="M61" s="20">
         <v>3</v>
       </c>
-      <c r="N61" s="28">
+      <c r="N61" s="21">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="P61" s="27">
+      <c r="P61" s="20">
         <v>3</v>
       </c>
-      <c r="Q61" s="28">
+      <c r="Q61" s="21">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="S61" s="8">
@@ -7910,40 +8917,40 @@
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A62" s="27">
+      <c r="A62" s="20">
         <v>4</v>
       </c>
-      <c r="B62" s="28">
+      <c r="B62" s="21">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="D62" s="27">
+      <c r="D62" s="20">
         <v>4</v>
       </c>
-      <c r="E62" s="28">
+      <c r="E62" s="21">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="G62" s="27">
+      <c r="G62" s="20">
         <v>4</v>
       </c>
-      <c r="H62" s="28">
+      <c r="H62" s="21">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J62" s="27">
+      <c r="J62" s="20">
         <v>4</v>
       </c>
-      <c r="K62" s="28">
+      <c r="K62" s="21">
         <v>5.67E-2</v>
       </c>
-      <c r="M62" s="27">
+      <c r="M62" s="20">
         <v>4</v>
       </c>
-      <c r="N62" s="28">
+      <c r="N62" s="21">
         <v>0.1132</v>
       </c>
-      <c r="P62" s="27">
+      <c r="P62" s="20">
         <v>4</v>
       </c>
-      <c r="Q62" s="28">
+      <c r="Q62" s="21">
         <v>3.4200000000000001E-2</v>
       </c>
       <c r="S62" s="8">
@@ -7955,40 +8962,40 @@
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A63" s="27">
+      <c r="A63" s="20">
         <v>5</v>
       </c>
-      <c r="B63" s="28">
+      <c r="B63" s="21">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D63" s="27">
+      <c r="D63" s="20">
         <v>5</v>
       </c>
-      <c r="E63" s="28">
+      <c r="E63" s="21">
         <v>1.06E-2</v>
       </c>
-      <c r="G63" s="27">
+      <c r="G63" s="20">
         <v>5</v>
       </c>
-      <c r="H63" s="28">
+      <c r="H63" s="21">
         <v>2.58E-2</v>
       </c>
-      <c r="J63" s="27">
+      <c r="J63" s="20">
         <v>5</v>
       </c>
-      <c r="K63" s="28">
+      <c r="K63" s="21">
         <v>5.7799999999999997E-2</v>
       </c>
-      <c r="M63" s="27">
+      <c r="M63" s="20">
         <v>5</v>
       </c>
-      <c r="N63" s="28">
+      <c r="N63" s="21">
         <v>4.5600000000000002E-2</v>
       </c>
-      <c r="P63" s="27">
+      <c r="P63" s="20">
         <v>5</v>
       </c>
-      <c r="Q63" s="28">
+      <c r="Q63" s="21">
         <v>0.2072</v>
       </c>
       <c r="S63" s="8">
@@ -8000,40 +9007,40 @@
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A64" s="27">
+      <c r="A64" s="20">
         <v>6</v>
       </c>
-      <c r="B64" s="28">
+      <c r="B64" s="21">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="D64" s="27">
+      <c r="D64" s="20">
         <v>6</v>
       </c>
-      <c r="E64" s="28">
+      <c r="E64" s="21">
         <v>5.4000000000000003E-3</v>
       </c>
-      <c r="G64" s="27">
+      <c r="G64" s="20">
         <v>6</v>
       </c>
-      <c r="H64" s="28">
+      <c r="H64" s="21">
         <v>6.3E-2</v>
       </c>
-      <c r="J64" s="27">
+      <c r="J64" s="20">
         <v>6</v>
       </c>
-      <c r="K64" s="28">
+      <c r="K64" s="21">
         <v>0.1114</v>
       </c>
-      <c r="M64" s="27">
+      <c r="M64" s="20">
         <v>6</v>
       </c>
-      <c r="N64" s="28">
+      <c r="N64" s="21">
         <v>3.9100000000000003E-2</v>
       </c>
-      <c r="P64" s="27">
+      <c r="P64" s="20">
         <v>6</v>
       </c>
-      <c r="Q64" s="28">
+      <c r="Q64" s="21">
         <v>0.10580000000000001</v>
       </c>
       <c r="S64" s="12">
@@ -8045,40 +9052,40 @@
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A65" s="27">
+      <c r="A65" s="20">
         <v>7</v>
       </c>
-      <c r="B65" s="28">
+      <c r="B65" s="21">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D65" s="27">
+      <c r="D65" s="20">
         <v>7</v>
       </c>
-      <c r="E65" s="28">
+      <c r="E65" s="21">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="G65" s="27">
+      <c r="G65" s="20">
         <v>7</v>
       </c>
-      <c r="H65" s="28">
+      <c r="H65" s="21">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="J65" s="27">
+      <c r="J65" s="20">
         <v>7</v>
       </c>
-      <c r="K65" s="28">
+      <c r="K65" s="21">
         <v>1.23E-2</v>
       </c>
-      <c r="M65" s="27">
+      <c r="M65" s="20">
         <v>7</v>
       </c>
-      <c r="N65" s="28">
+      <c r="N65" s="21">
         <v>2.64E-2</v>
       </c>
-      <c r="P65" s="27">
+      <c r="P65" s="20">
         <v>7</v>
       </c>
-      <c r="Q65" s="28">
+      <c r="Q65" s="21">
         <v>6.0699999999999997E-2</v>
       </c>
       <c r="S65" s="8">
@@ -8090,40 +9097,40 @@
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A66" s="27">
+      <c r="A66" s="20">
         <v>8</v>
       </c>
-      <c r="B66" s="28">
+      <c r="B66" s="21">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="D66" s="27">
+      <c r="D66" s="20">
         <v>8</v>
       </c>
-      <c r="E66" s="28">
+      <c r="E66" s="21">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="G66" s="27">
+      <c r="G66" s="20">
         <v>8</v>
       </c>
-      <c r="H66" s="28">
+      <c r="H66" s="21">
         <v>5.6099999999999997E-2</v>
       </c>
-      <c r="J66" s="27">
+      <c r="J66" s="20">
         <v>8</v>
       </c>
-      <c r="K66" s="28">
+      <c r="K66" s="21">
         <v>6.2799999999999995E-2</v>
       </c>
-      <c r="M66" s="27">
+      <c r="M66" s="20">
         <v>8</v>
       </c>
-      <c r="N66" s="28">
+      <c r="N66" s="21">
         <v>7.1499999999999994E-2</v>
       </c>
-      <c r="P66" s="27">
+      <c r="P66" s="20">
         <v>8</v>
       </c>
-      <c r="Q66" s="28">
+      <c r="Q66" s="21">
         <v>0.13139999999999999</v>
       </c>
       <c r="S66" s="8">
@@ -8135,142 +9142,679 @@
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A67" s="27">
+      <c r="A67" s="20">
         <v>9</v>
       </c>
-      <c r="B67" s="28">
+      <c r="B67" s="21">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D67" s="27">
+      <c r="D67" s="20">
         <v>9</v>
       </c>
-      <c r="E67" s="28">
+      <c r="E67" s="21">
         <v>6.1000000000000004E-3</v>
       </c>
-      <c r="G67" s="27">
+      <c r="G67" s="20">
         <v>9</v>
       </c>
-      <c r="H67" s="28">
+      <c r="H67" s="21">
         <v>8.5400000000000004E-2</v>
       </c>
-      <c r="J67" s="27">
+      <c r="J67" s="20">
         <v>9</v>
       </c>
-      <c r="K67" s="28">
+      <c r="K67" s="21">
         <v>0.1295</v>
       </c>
-      <c r="M67" s="27">
+      <c r="M67" s="20">
         <v>9</v>
       </c>
-      <c r="N67" s="28">
+      <c r="N67" s="21">
         <v>5.2699999999999997E-2</v>
       </c>
-      <c r="P67" s="27">
+      <c r="P67" s="20">
         <v>9</v>
       </c>
-      <c r="Q67" s="28">
+      <c r="Q67" s="21">
         <v>1.5100000000000001E-2</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A68" s="27">
+      <c r="A68" s="20">
         <v>10</v>
       </c>
-      <c r="B68" s="28">
+      <c r="B68" s="21">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="D68" s="27">
+      <c r="D68" s="20">
         <v>10</v>
       </c>
-      <c r="E68" s="28">
+      <c r="E68" s="21">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="G68" s="27">
+      <c r="G68" s="20">
         <v>10</v>
       </c>
-      <c r="H68" s="28">
+      <c r="H68" s="21">
         <v>6.4600000000000005E-2</v>
       </c>
-      <c r="J68" s="27">
+      <c r="J68" s="20">
         <v>10</v>
       </c>
-      <c r="K68" s="28">
+      <c r="K68" s="21">
         <v>7.0400000000000004E-2</v>
       </c>
-      <c r="M68" s="27">
+      <c r="M68" s="20">
         <v>10</v>
       </c>
-      <c r="N68" s="28">
+      <c r="N68" s="21">
         <v>8.6900000000000005E-2</v>
       </c>
-      <c r="P68" s="27">
+      <c r="P68" s="20">
         <v>10</v>
       </c>
-      <c r="Q68" s="28">
+      <c r="Q68" s="21">
         <v>5.7599999999999998E-2</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A69" s="27" t="s">
+      <c r="A69" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B69" s="27">
+      <c r="B69" s="20">
         <f>AVERAGE(B59:B68)</f>
         <v>5.3579999999999975E-2</v>
       </c>
-      <c r="D69" s="27" t="s">
+      <c r="D69" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E69" s="27">
+      <c r="E69" s="20">
         <f>AVERAGE(E59:E68)</f>
         <v>5.7129999999999993E-2</v>
       </c>
-      <c r="G69" s="27" t="s">
+      <c r="G69" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H69" s="27">
+      <c r="H69" s="20">
         <f>AVERAGE(H59:H68)</f>
         <v>9.7689999999999999E-2</v>
       </c>
-      <c r="J69" s="27" t="s">
+      <c r="J69" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K69" s="27">
+      <c r="K69" s="20">
         <f>AVERAGE(K59:K68)</f>
         <v>0.11685999999999999</v>
       </c>
-      <c r="M69" s="27" t="s">
+      <c r="M69" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="N69" s="27">
+      <c r="N69" s="20">
         <f>AVERAGE(N59:N68)</f>
         <v>0.15751999999999997</v>
       </c>
-      <c r="P69" s="27" t="s">
+      <c r="P69" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="Q69" s="27">
+      <c r="Q69" s="20">
         <f>AVERAGE(Q59:Q68)</f>
         <v>0.15762999999999999</v>
       </c>
     </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A71" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71" s="29"/>
+      <c r="D71" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" s="29"/>
+      <c r="G71" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="H71" s="29"/>
+      <c r="J71" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="K71" s="29"/>
+      <c r="M71" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="N71" s="29"/>
+      <c r="P71" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q71" s="29"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A72" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G72" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="H72" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="J72" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="K72" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M72" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="N72" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="P72" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A73" s="30">
+        <v>1</v>
+      </c>
+      <c r="B73" s="31">
+        <v>0.12609999999999999</v>
+      </c>
+      <c r="D73" s="30">
+        <v>1</v>
+      </c>
+      <c r="E73" s="31">
+        <v>0.1275</v>
+      </c>
+      <c r="G73" s="30">
+        <v>1</v>
+      </c>
+      <c r="H73" s="31">
+        <v>0.15290000000000001</v>
+      </c>
+      <c r="J73" s="30">
+        <v>1</v>
+      </c>
+      <c r="K73" s="31">
+        <v>0.1699</v>
+      </c>
+      <c r="M73" s="30">
+        <v>1</v>
+      </c>
+      <c r="N73" s="31">
+        <v>0.20830000000000001</v>
+      </c>
+      <c r="P73" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="31">
+        <v>0.2419</v>
+      </c>
+      <c r="S73" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="T73" s="24"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A74" s="30">
+        <v>2</v>
+      </c>
+      <c r="B74" s="31">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D74" s="30">
+        <v>2</v>
+      </c>
+      <c r="E74" s="31">
+        <v>1.5E-3</v>
+      </c>
+      <c r="G74" s="30">
+        <v>2</v>
+      </c>
+      <c r="H74" s="31">
+        <v>8.6E-3</v>
+      </c>
+      <c r="J74" s="30">
+        <v>2</v>
+      </c>
+      <c r="K74" s="31">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="M74" s="30">
+        <v>2</v>
+      </c>
+      <c r="N74" s="31">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="P74" s="30">
+        <v>2</v>
+      </c>
+      <c r="Q74" s="31">
+        <v>9.7600000000000006E-2</v>
+      </c>
+      <c r="S74" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T74" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A75" s="30">
+        <v>3</v>
+      </c>
+      <c r="B75" s="31">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D75" s="30">
+        <v>3</v>
+      </c>
+      <c r="E75" s="31">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="G75" s="30">
+        <v>3</v>
+      </c>
+      <c r="H75" s="31">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="J75" s="30">
+        <v>3</v>
+      </c>
+      <c r="K75" s="31">
+        <v>3.2599999999999997E-2</v>
+      </c>
+      <c r="M75" s="30">
+        <v>3</v>
+      </c>
+      <c r="N75" s="31">
+        <v>5.5500000000000001E-2</v>
+      </c>
+      <c r="P75" s="30">
+        <v>3</v>
+      </c>
+      <c r="Q75" s="31">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="S75" s="8">
+        <v>10</v>
+      </c>
+      <c r="T75" s="8">
+        <f>B83</f>
+        <v>1.3590000000000001E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A76" s="30">
+        <v>4</v>
+      </c>
+      <c r="B76" s="31">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D76" s="30">
+        <v>4</v>
+      </c>
+      <c r="E76" s="31">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="G76" s="30">
+        <v>4</v>
+      </c>
+      <c r="H76" s="31">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J76" s="30">
+        <v>4</v>
+      </c>
+      <c r="K76" s="31">
+        <v>2.47E-2</v>
+      </c>
+      <c r="M76" s="30">
+        <v>4</v>
+      </c>
+      <c r="N76" s="31">
+        <v>5.04E-2</v>
+      </c>
+      <c r="P76" s="30">
+        <v>4</v>
+      </c>
+      <c r="Q76" s="31">
+        <v>0.1148</v>
+      </c>
+      <c r="S76" s="8">
+        <v>100</v>
+      </c>
+      <c r="T76" s="8">
+        <f>E83</f>
+        <v>1.396E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A77" s="30">
+        <v>5</v>
+      </c>
+      <c r="B77" s="31">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D77" s="30">
+        <v>5</v>
+      </c>
+      <c r="E77" s="31">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="G77" s="30">
+        <v>5</v>
+      </c>
+      <c r="H77" s="31">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="J77" s="30">
+        <v>5</v>
+      </c>
+      <c r="K77" s="31">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="M77" s="30">
+        <v>5</v>
+      </c>
+      <c r="N77" s="31">
+        <v>5.2299999999999999E-2</v>
+      </c>
+      <c r="P77" s="30">
+        <v>5</v>
+      </c>
+      <c r="Q77" s="31">
+        <v>0.10630000000000001</v>
+      </c>
+      <c r="S77" s="8">
+        <v>1000</v>
+      </c>
+      <c r="T77" s="8">
+        <f>H83</f>
+        <v>2.155E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A78" s="30">
+        <v>6</v>
+      </c>
+      <c r="B78" s="31">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="D78" s="30">
+        <v>6</v>
+      </c>
+      <c r="E78" s="31">
+        <v>1.5E-3</v>
+      </c>
+      <c r="G78" s="30">
+        <v>6</v>
+      </c>
+      <c r="H78" s="31">
+        <v>1.12E-2</v>
+      </c>
+      <c r="J78" s="30">
+        <v>6</v>
+      </c>
+      <c r="K78" s="31">
+        <v>2.75E-2</v>
+      </c>
+      <c r="M78" s="30">
+        <v>6</v>
+      </c>
+      <c r="N78" s="31">
+        <v>5.5399999999999998E-2</v>
+      </c>
+      <c r="P78" s="30">
+        <v>6</v>
+      </c>
+      <c r="Q78" s="31">
+        <v>6.1800000000000001E-2</v>
+      </c>
+      <c r="S78" s="12">
+        <v>5000</v>
+      </c>
+      <c r="T78" s="12">
+        <f>K83</f>
+        <v>4.1149999999999999E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A79" s="30">
+        <v>7</v>
+      </c>
+      <c r="B79" s="31">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="D79" s="30">
+        <v>7</v>
+      </c>
+      <c r="E79" s="31">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="G79" s="30">
+        <v>7</v>
+      </c>
+      <c r="H79" s="31">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="J79" s="30">
+        <v>7</v>
+      </c>
+      <c r="K79" s="31">
+        <v>2.7699999999999999E-2</v>
+      </c>
+      <c r="M79" s="30">
+        <v>7</v>
+      </c>
+      <c r="N79" s="31">
+        <v>5.7299999999999997E-2</v>
+      </c>
+      <c r="P79" s="30">
+        <v>7</v>
+      </c>
+      <c r="Q79" s="31">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="S79" s="8">
+        <v>10000</v>
+      </c>
+      <c r="T79" s="8">
+        <f>N83</f>
+        <v>6.1760000000000002E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A80" s="30">
+        <v>8</v>
+      </c>
+      <c r="B80" s="31">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D80" s="30">
+        <v>8</v>
+      </c>
+      <c r="E80" s="31">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="G80" s="30">
+        <v>8</v>
+      </c>
+      <c r="H80" s="31">
+        <v>7.6E-3</v>
+      </c>
+      <c r="J80" s="30">
+        <v>8</v>
+      </c>
+      <c r="K80" s="31">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="M80" s="30">
+        <v>8</v>
+      </c>
+      <c r="N80" s="31">
+        <v>3.0099999999999998E-2</v>
+      </c>
+      <c r="P80" s="30">
+        <v>8</v>
+      </c>
+      <c r="Q80" s="31">
+        <v>7.4099999999999999E-2</v>
+      </c>
+      <c r="S80" s="8">
+        <v>20000</v>
+      </c>
+      <c r="T80" s="8">
+        <f>Q83</f>
+        <v>9.9099999999999994E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A81" s="30">
+        <v>9</v>
+      </c>
+      <c r="B81" s="31">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D81" s="30">
+        <v>9</v>
+      </c>
+      <c r="E81" s="31">
+        <v>1.5E-3</v>
+      </c>
+      <c r="G81" s="30">
+        <v>9</v>
+      </c>
+      <c r="H81" s="31">
+        <v>7.6E-3</v>
+      </c>
+      <c r="J81" s="30">
+        <v>9</v>
+      </c>
+      <c r="K81" s="31">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="M81" s="30">
+        <v>9</v>
+      </c>
+      <c r="N81" s="31">
+        <v>3.0200000000000001E-2</v>
+      </c>
+      <c r="P81" s="30">
+        <v>9</v>
+      </c>
+      <c r="Q81" s="31">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A82" s="30">
+        <v>10</v>
+      </c>
+      <c r="B82" s="31">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D82" s="30">
+        <v>10</v>
+      </c>
+      <c r="E82" s="31">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="G82" s="30">
+        <v>10</v>
+      </c>
+      <c r="H82" s="31">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="J82" s="30">
+        <v>10</v>
+      </c>
+      <c r="K82" s="31">
+        <v>1.67E-2</v>
+      </c>
+      <c r="M82" s="30">
+        <v>10</v>
+      </c>
+      <c r="N82" s="31">
+        <v>2.98E-2</v>
+      </c>
+      <c r="P82" s="30">
+        <v>10</v>
+      </c>
+      <c r="Q82" s="31">
+        <v>5.8999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A83" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B83" s="30">
+        <f>AVERAGE(B73:B82)</f>
+        <v>1.3590000000000001E-2</v>
+      </c>
+      <c r="D83" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E83" s="30">
+        <f>AVERAGE(E73:E82)</f>
+        <v>1.396E-2</v>
+      </c>
+      <c r="G83" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="H83" s="30">
+        <f>AVERAGE(H73:H82)</f>
+        <v>2.155E-2</v>
+      </c>
+      <c r="J83" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="K83" s="30">
+        <f>AVERAGE(K73:K82)</f>
+        <v>4.1149999999999999E-2</v>
+      </c>
+      <c r="M83" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="N83" s="30">
+        <f>AVERAGE(N73:N82)</f>
+        <v>6.1760000000000002E-2</v>
+      </c>
+      <c r="P83" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q83" s="30">
+        <f>AVERAGE(Q73:Q82)</f>
+        <v>9.9099999999999994E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="S59:T59"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="M15:N15"/>
+  <mergeCells count="42">
+    <mergeCell ref="P71:Q71"/>
+    <mergeCell ref="S73:T73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="M71:N71"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P29:Q29"/>
     <mergeCell ref="S45:T45"/>
     <mergeCell ref="S31:T31"/>
     <mergeCell ref="A43:B43"/>
@@ -8282,15 +9826,25 @@
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="M29:N29"/>
     <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="M15:N15"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="S59:T59"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="M57:N57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8300,8 +9854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E1DFA1C-B479-9845-B834-AC124B3DC7B7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added ShuffleArray method with timings
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissasedgwick/Projects/Makers/Week_10/algorithmic-complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2839EA5-86F8-E74C-90D5-2A3A1784C5D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5869518-DDB7-9447-94E1-55E5B81DD369}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-10500" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{0EC00D74-CF7F-6E46-A448-9AC86E039AD3}"/>
   </bookViews>
@@ -17,10 +17,10 @@
     <sheet name="Graphs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.2" hidden="1">Data!$S$75:$S$80</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Data!$T$75:$T$80</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Data!$S$75:$S$80</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Data!$T$75:$T$80</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Data!$S$89:$S$94</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Data!$T$89:$T$94</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Data!$S$89:$S$94</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Data!$T$89:$T$94</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="48">
   <si>
     <t>Attempt</t>
   </si>
@@ -159,6 +159,24 @@
   <si>
     <t>Own Reverse on List of length 20000</t>
   </si>
+  <si>
+    <t>Own ShuffleArray on List of length 10</t>
+  </si>
+  <si>
+    <t>Own ShuffleArray on List of length 100</t>
+  </si>
+  <si>
+    <t>Own ShuffleArray on List of length 1000</t>
+  </si>
+  <si>
+    <t>Own ShuffleArray on List of length 5000</t>
+  </si>
+  <si>
+    <t>Own ShuffleArray on List of length 10000</t>
+  </si>
+  <si>
+    <t>Own ShuffleArray on List of length 20000</t>
+  </si>
 </sst>
 </file>
 
@@ -173,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +231,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBE77FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF41A08E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -334,6 +358,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,6 +371,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF41A08E"/>
       <color rgb="FFBE77FF"/>
       <color rgb="FFFFB4E3"/>
     </mruColors>
@@ -2504,6 +2534,367 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ShuffleArray -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Own Method</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$S$89:$S$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$T$89:$T$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.6269999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22457000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9269400000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1548700000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.372859999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.433230000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C4BF-7C4B-B376-C59BC13F2F50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1666620944"/>
+        <c:axId val="1686407552"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1666620944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1686407552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1686407552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1666620944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2744,6 +3135,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -5435,6 +5866,544 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6202,6 +7171,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D934EAA-D556-BD4F-8341-DF9DA0219823}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6502,10 +7509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D4128A-2966-F54D-A276-45E672D85F83}">
-  <dimension ref="A1:T83"/>
+  <dimension ref="A1:T97"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="T80" sqref="S75:T80"/>
+    <sheetView topLeftCell="B62" workbookViewId="0">
+      <selection activeCell="S89" sqref="S89:T94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9681,7 +10688,7 @@
         <v>9.9099999999999994E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="30">
         <v>9</v>
       </c>
@@ -9719,7 +10726,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="30">
         <v>10</v>
       </c>
@@ -9757,7 +10764,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="30" t="s">
         <v>1</v>
       </c>
@@ -9801,10 +10808,557 @@
         <v>9.9099999999999994E-2</v>
       </c>
     </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A85" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" s="32"/>
+      <c r="D85" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E85" s="32"/>
+      <c r="G85" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="H85" s="32"/>
+      <c r="J85" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="K85" s="32"/>
+      <c r="M85" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="N85" s="32"/>
+      <c r="P85" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q85" s="32"/>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A86" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G86" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="H86" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="J86" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="K86" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="M86" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="N86" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="P86" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q86" s="33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A87" s="33">
+        <v>1</v>
+      </c>
+      <c r="B87" s="34">
+        <v>0.23150000000000001</v>
+      </c>
+      <c r="D87" s="33">
+        <v>1</v>
+      </c>
+      <c r="E87" s="34">
+        <v>0.46360000000000001</v>
+      </c>
+      <c r="G87" s="33">
+        <v>1</v>
+      </c>
+      <c r="H87" s="34">
+        <v>2.8283</v>
+      </c>
+      <c r="J87" s="33">
+        <v>1</v>
+      </c>
+      <c r="K87" s="34">
+        <v>9.3878000000000004</v>
+      </c>
+      <c r="M87" s="33">
+        <v>1</v>
+      </c>
+      <c r="N87" s="34">
+        <v>18.275300000000001</v>
+      </c>
+      <c r="P87" s="33">
+        <v>1</v>
+      </c>
+      <c r="Q87" s="34">
+        <v>35.527700000000003</v>
+      </c>
+      <c r="S87" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="T87" s="24"/>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A88" s="33">
+        <v>2</v>
+      </c>
+      <c r="B88" s="34">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="D88" s="33">
+        <v>2</v>
+      </c>
+      <c r="E88" s="34">
+        <v>0.1764</v>
+      </c>
+      <c r="G88" s="33">
+        <v>2</v>
+      </c>
+      <c r="H88" s="34">
+        <v>1.7728999999999999</v>
+      </c>
+      <c r="J88" s="33">
+        <v>2</v>
+      </c>
+      <c r="K88" s="34">
+        <v>9.2772000000000006</v>
+      </c>
+      <c r="M88" s="33">
+        <v>2</v>
+      </c>
+      <c r="N88" s="34">
+        <v>17.625599999999999</v>
+      </c>
+      <c r="P88" s="33">
+        <v>2</v>
+      </c>
+      <c r="Q88" s="34">
+        <v>35.668500000000002</v>
+      </c>
+      <c r="S88" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T88" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A89" s="33">
+        <v>3</v>
+      </c>
+      <c r="B89" s="34">
+        <v>1.84E-2</v>
+      </c>
+      <c r="D89" s="33">
+        <v>3</v>
+      </c>
+      <c r="E89" s="34">
+        <v>0.1956</v>
+      </c>
+      <c r="G89" s="33">
+        <v>3</v>
+      </c>
+      <c r="H89" s="34">
+        <v>1.7262999999999999</v>
+      </c>
+      <c r="J89" s="33">
+        <v>3</v>
+      </c>
+      <c r="K89" s="34">
+        <v>9.5783000000000005</v>
+      </c>
+      <c r="M89" s="33">
+        <v>3</v>
+      </c>
+      <c r="N89" s="34">
+        <v>17.778700000000001</v>
+      </c>
+      <c r="P89" s="33">
+        <v>3</v>
+      </c>
+      <c r="Q89" s="34">
+        <v>37.237900000000003</v>
+      </c>
+      <c r="S89" s="8">
+        <v>10</v>
+      </c>
+      <c r="T89" s="8">
+        <f>B97</f>
+        <v>4.6269999999999992E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A90" s="33">
+        <v>4</v>
+      </c>
+      <c r="B90" s="34">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="D90" s="33">
+        <v>4</v>
+      </c>
+      <c r="E90" s="34">
+        <v>0.20569999999999999</v>
+      </c>
+      <c r="G90" s="33">
+        <v>4</v>
+      </c>
+      <c r="H90" s="34">
+        <v>1.9536</v>
+      </c>
+      <c r="J90" s="33">
+        <v>4</v>
+      </c>
+      <c r="K90" s="34">
+        <v>9.1522000000000006</v>
+      </c>
+      <c r="M90" s="33">
+        <v>4</v>
+      </c>
+      <c r="N90" s="34">
+        <v>17.869700000000002</v>
+      </c>
+      <c r="P90" s="33">
+        <v>4</v>
+      </c>
+      <c r="Q90" s="34">
+        <v>35.847200000000001</v>
+      </c>
+      <c r="S90" s="8">
+        <v>100</v>
+      </c>
+      <c r="T90" s="8">
+        <f>E97</f>
+        <v>0.22457000000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A91" s="33">
+        <v>5</v>
+      </c>
+      <c r="B91" s="34">
+        <v>2.4899999999999999E-2</v>
+      </c>
+      <c r="D91" s="33">
+        <v>5</v>
+      </c>
+      <c r="E91" s="34">
+        <v>0.19309999999999999</v>
+      </c>
+      <c r="G91" s="33">
+        <v>5</v>
+      </c>
+      <c r="H91" s="34">
+        <v>1.85</v>
+      </c>
+      <c r="J91" s="33">
+        <v>5</v>
+      </c>
+      <c r="K91" s="34">
+        <v>9.1341000000000001</v>
+      </c>
+      <c r="M91" s="33">
+        <v>5</v>
+      </c>
+      <c r="N91" s="34">
+        <v>17.877800000000001</v>
+      </c>
+      <c r="P91" s="33">
+        <v>5</v>
+      </c>
+      <c r="Q91" s="34">
+        <v>33.704599999999999</v>
+      </c>
+      <c r="S91" s="8">
+        <v>1000</v>
+      </c>
+      <c r="T91" s="8">
+        <f>H97</f>
+        <v>1.9269400000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A92" s="33">
+        <v>6</v>
+      </c>
+      <c r="B92" s="34">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="D92" s="33">
+        <v>6</v>
+      </c>
+      <c r="E92" s="34">
+        <v>0.1973</v>
+      </c>
+      <c r="G92" s="33">
+        <v>6</v>
+      </c>
+      <c r="H92" s="34">
+        <v>1.7258</v>
+      </c>
+      <c r="J92" s="33">
+        <v>6</v>
+      </c>
+      <c r="K92" s="34">
+        <v>9.2393999999999998</v>
+      </c>
+      <c r="M92" s="33">
+        <v>6</v>
+      </c>
+      <c r="N92" s="34">
+        <v>17.426200000000001</v>
+      </c>
+      <c r="P92" s="33">
+        <v>6</v>
+      </c>
+      <c r="Q92" s="34">
+        <v>33.746000000000002</v>
+      </c>
+      <c r="S92" s="12">
+        <v>5000</v>
+      </c>
+      <c r="T92" s="12">
+        <f>K97</f>
+        <v>9.1548700000000007</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A93" s="33">
+        <v>7</v>
+      </c>
+      <c r="B93" s="34">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="D93" s="33">
+        <v>7</v>
+      </c>
+      <c r="E93" s="34">
+        <v>0.19550000000000001</v>
+      </c>
+      <c r="G93" s="33">
+        <v>7</v>
+      </c>
+      <c r="H93" s="34">
+        <v>1.8489</v>
+      </c>
+      <c r="J93" s="33">
+        <v>7</v>
+      </c>
+      <c r="K93" s="34">
+        <v>9.0716000000000001</v>
+      </c>
+      <c r="M93" s="33">
+        <v>7</v>
+      </c>
+      <c r="N93" s="34">
+        <v>16.725100000000001</v>
+      </c>
+      <c r="P93" s="33">
+        <v>7</v>
+      </c>
+      <c r="Q93" s="34">
+        <v>33.805399999999999</v>
+      </c>
+      <c r="S93" s="8">
+        <v>10000</v>
+      </c>
+      <c r="T93" s="8">
+        <f>N97</f>
+        <v>17.372859999999996</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A94" s="33">
+        <v>8</v>
+      </c>
+      <c r="B94" s="34">
+        <v>2.3900000000000001E-2</v>
+      </c>
+      <c r="D94" s="33">
+        <v>8</v>
+      </c>
+      <c r="E94" s="34">
+        <v>0.2243</v>
+      </c>
+      <c r="G94" s="33">
+        <v>8</v>
+      </c>
+      <c r="H94" s="34">
+        <v>1.8979999999999999</v>
+      </c>
+      <c r="J94" s="33">
+        <v>8</v>
+      </c>
+      <c r="K94" s="34">
+        <v>9.6374999999999993</v>
+      </c>
+      <c r="M94" s="33">
+        <v>8</v>
+      </c>
+      <c r="N94" s="34">
+        <v>16.620999999999999</v>
+      </c>
+      <c r="P94" s="33">
+        <v>8</v>
+      </c>
+      <c r="Q94" s="34">
+        <v>32.347200000000001</v>
+      </c>
+      <c r="S94" s="8">
+        <v>20000</v>
+      </c>
+      <c r="T94" s="8">
+        <f>Q97</f>
+        <v>34.433230000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A95" s="33">
+        <v>9</v>
+      </c>
+      <c r="B95" s="34">
+        <v>1.66E-2</v>
+      </c>
+      <c r="D95" s="33">
+        <v>9</v>
+      </c>
+      <c r="E95" s="34">
+        <v>0.19089999999999999</v>
+      </c>
+      <c r="G95" s="33">
+        <v>9</v>
+      </c>
+      <c r="H95" s="34">
+        <v>1.7193000000000001</v>
+      </c>
+      <c r="J95" s="33">
+        <v>9</v>
+      </c>
+      <c r="K95" s="34">
+        <v>8.5372000000000003</v>
+      </c>
+      <c r="M95" s="33">
+        <v>9</v>
+      </c>
+      <c r="N95" s="34">
+        <v>16.603200000000001</v>
+      </c>
+      <c r="P95" s="33">
+        <v>9</v>
+      </c>
+      <c r="Q95" s="34">
+        <v>33.009500000000003</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A96" s="33">
+        <v>10</v>
+      </c>
+      <c r="B96" s="34">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="D96" s="33">
+        <v>10</v>
+      </c>
+      <c r="E96" s="34">
+        <v>0.20330000000000001</v>
+      </c>
+      <c r="G96" s="33">
+        <v>10</v>
+      </c>
+      <c r="H96" s="34">
+        <v>1.9462999999999999</v>
+      </c>
+      <c r="J96" s="33">
+        <v>10</v>
+      </c>
+      <c r="K96" s="34">
+        <v>8.5334000000000003</v>
+      </c>
+      <c r="M96" s="33">
+        <v>10</v>
+      </c>
+      <c r="N96" s="34">
+        <v>16.925999999999998</v>
+      </c>
+      <c r="P96" s="33">
+        <v>10</v>
+      </c>
+      <c r="Q96" s="34">
+        <v>33.438299999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A97" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B97" s="33">
+        <f>AVERAGE(B87:B96)</f>
+        <v>4.6269999999999992E-2</v>
+      </c>
+      <c r="D97" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E97" s="33">
+        <f>AVERAGE(E87:E96)</f>
+        <v>0.22457000000000002</v>
+      </c>
+      <c r="G97" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="H97" s="33">
+        <f>AVERAGE(H87:H96)</f>
+        <v>1.9269400000000001</v>
+      </c>
+      <c r="J97" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="K97" s="33">
+        <f>AVERAGE(K87:K96)</f>
+        <v>9.1548700000000007</v>
+      </c>
+      <c r="M97" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="N97" s="33">
+        <f>AVERAGE(N87:N96)</f>
+        <v>17.372859999999996</v>
+      </c>
+      <c r="P97" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q97" s="33">
+        <f>AVERAGE(Q87:Q96)</f>
+        <v>34.433230000000002</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="49">
+    <mergeCell ref="S87:T87"/>
     <mergeCell ref="P71:Q71"/>
     <mergeCell ref="S73:T73"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="J85:K85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="G71:H71"/>
@@ -9855,7 +11409,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added timings for Pairing method
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissasedgwick/Projects/Makers/Week_10/algorithmic-complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5869518-DDB7-9447-94E1-55E5B81DD369}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3628FBBA-79F4-CC48-A6D0-E9D210B0B9B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-10500" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{0EC00D74-CF7F-6E46-A448-9AC86E039AD3}"/>
   </bookViews>
@@ -17,10 +17,10 @@
     <sheet name="Graphs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Data!$S$89:$S$94</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Data!$T$89:$T$94</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Data!$S$89:$S$94</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Data!$T$89:$T$94</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Data!$S$103:$S$108</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Data!$T$103:$T$108</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Data!$S$103:$S$108</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Data!$T$103:$T$108</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="54">
   <si>
     <t>Attempt</t>
   </si>
@@ -177,6 +177,24 @@
   <si>
     <t>Own ShuffleArray on List of length 20000</t>
   </si>
+  <si>
+    <t>Own Pairing on List of length 10</t>
+  </si>
+  <si>
+    <t>Own Pairing on List of length 100</t>
+  </si>
+  <si>
+    <t>Own Pairing on List of length 1000</t>
+  </si>
+  <si>
+    <t>Own Pairing on List of length 5000</t>
+  </si>
+  <si>
+    <t>Own Pairing on List of length 10000</t>
+  </si>
+  <si>
+    <t>Own Pairing on List of length 20000</t>
+  </si>
 </sst>
 </file>
 
@@ -191,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,6 +255,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF41A08E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF45A8C1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -363,6 +387,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,6 +400,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF45A8C1"/>
       <color rgb="FF41A08E"/>
       <color rgb="FFBE77FF"/>
       <color rgb="FFFFB4E3"/>
@@ -2895,6 +2925,368 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Pairing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Own Method</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$S$103:$S$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$T$103:$T$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.0789999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27732000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.554299999999984</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1950.5017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11241.370299999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58660.935979999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2138-274A-BF49-0F7948FBCB9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1631822128"/>
+        <c:axId val="1669296352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1631822128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1669296352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1669296352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="65000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1631822128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3175,6 +3567,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -6404,6 +6836,544 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7209,6 +8179,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FCF3A38-D3D6-A945-92B7-871B3562F216}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7509,10 +8517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D4128A-2966-F54D-A276-45E672D85F83}">
-  <dimension ref="A1:T97"/>
+  <dimension ref="A1:T111"/>
   <sheetViews>
-    <sheetView topLeftCell="B62" workbookViewId="0">
-      <selection activeCell="S89" sqref="S89:T94"/>
+    <sheetView topLeftCell="D78" workbookViewId="0">
+      <selection activeCell="S103" sqref="S103:T108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11304,7 +12312,7 @@
         <v>33.438299999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97" s="33" t="s">
         <v>1</v>
       </c>
@@ -11348,9 +12356,556 @@
         <v>34.433230000000002</v>
       </c>
     </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A99" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B99" s="35"/>
+      <c r="D99" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E99" s="35"/>
+      <c r="G99" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="H99" s="35"/>
+      <c r="J99" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="K99" s="35"/>
+      <c r="M99" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="N99" s="35"/>
+      <c r="P99" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q99" s="35"/>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A100" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G100" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="H100" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="J100" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="K100" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="M100" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="N100" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="P100" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q100" s="36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A101" s="36">
+        <v>1</v>
+      </c>
+      <c r="B101" s="37">
+        <v>0.26369999999999999</v>
+      </c>
+      <c r="D101" s="36">
+        <v>1</v>
+      </c>
+      <c r="E101" s="37">
+        <v>0.64170000000000005</v>
+      </c>
+      <c r="G101" s="36">
+        <v>1</v>
+      </c>
+      <c r="H101" s="37">
+        <v>48.407200000000003</v>
+      </c>
+      <c r="J101" s="36">
+        <v>1</v>
+      </c>
+      <c r="K101" s="37">
+        <v>1891.9315999999999</v>
+      </c>
+      <c r="M101" s="36">
+        <v>1</v>
+      </c>
+      <c r="N101" s="37">
+        <v>8529.7643000000007</v>
+      </c>
+      <c r="P101" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q101" s="37">
+        <v>58181.758199999997</v>
+      </c>
+      <c r="S101" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="T101" s="24"/>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A102" s="36">
+        <v>2</v>
+      </c>
+      <c r="B102" s="37">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="D102" s="36">
+        <v>2</v>
+      </c>
+      <c r="E102" s="37">
+        <v>0.3286</v>
+      </c>
+      <c r="G102" s="36">
+        <v>2</v>
+      </c>
+      <c r="H102" s="37">
+        <v>30.108899999999998</v>
+      </c>
+      <c r="J102" s="36">
+        <v>2</v>
+      </c>
+      <c r="K102" s="37">
+        <v>2170.3139000000001</v>
+      </c>
+      <c r="M102" s="36">
+        <v>2</v>
+      </c>
+      <c r="N102" s="37">
+        <v>7649.1914999999999</v>
+      </c>
+      <c r="P102" s="36">
+        <v>2</v>
+      </c>
+      <c r="Q102" s="37">
+        <v>53606.411200000002</v>
+      </c>
+      <c r="S102" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T102" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A103" s="36">
+        <v>3</v>
+      </c>
+      <c r="B103" s="37">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D103" s="36">
+        <v>3</v>
+      </c>
+      <c r="E103" s="37">
+        <v>0.32240000000000002</v>
+      </c>
+      <c r="G103" s="36">
+        <v>3</v>
+      </c>
+      <c r="H103" s="37">
+        <v>94.297399999999996</v>
+      </c>
+      <c r="J103" s="36">
+        <v>3</v>
+      </c>
+      <c r="K103" s="37">
+        <v>1531.8221000000001</v>
+      </c>
+      <c r="M103" s="36">
+        <v>3</v>
+      </c>
+      <c r="N103" s="37">
+        <v>10921.740400000001</v>
+      </c>
+      <c r="P103" s="36">
+        <v>3</v>
+      </c>
+      <c r="Q103" s="37">
+        <v>56379.284599999999</v>
+      </c>
+      <c r="S103" s="8">
+        <v>10</v>
+      </c>
+      <c r="T103" s="8">
+        <f>B111</f>
+        <v>3.0789999999999994E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A104" s="36">
+        <v>4</v>
+      </c>
+      <c r="B104" s="37">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="D104" s="36">
+        <v>4</v>
+      </c>
+      <c r="E104" s="37">
+        <v>0.31740000000000002</v>
+      </c>
+      <c r="G104" s="36">
+        <v>4</v>
+      </c>
+      <c r="H104" s="37">
+        <v>65.040899999999993</v>
+      </c>
+      <c r="J104" s="36">
+        <v>4</v>
+      </c>
+      <c r="K104" s="37">
+        <v>2695.6289999999999</v>
+      </c>
+      <c r="M104" s="36">
+        <v>4</v>
+      </c>
+      <c r="N104" s="37">
+        <v>11994.1513</v>
+      </c>
+      <c r="P104" s="36">
+        <v>4</v>
+      </c>
+      <c r="Q104" s="37">
+        <v>58123.683100000002</v>
+      </c>
+      <c r="S104" s="8">
+        <v>100</v>
+      </c>
+      <c r="T104" s="8">
+        <f>E111</f>
+        <v>0.27732000000000007</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A105" s="36">
+        <v>5</v>
+      </c>
+      <c r="B105" s="37">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D105" s="36">
+        <v>5</v>
+      </c>
+      <c r="E105" s="37">
+        <v>0.32990000000000003</v>
+      </c>
+      <c r="G105" s="36">
+        <v>5</v>
+      </c>
+      <c r="H105" s="37">
+        <v>91.207700000000003</v>
+      </c>
+      <c r="J105" s="36">
+        <v>5</v>
+      </c>
+      <c r="K105" s="37">
+        <v>2339.3253</v>
+      </c>
+      <c r="M105" s="36">
+        <v>5</v>
+      </c>
+      <c r="N105" s="37">
+        <v>12334.2952</v>
+      </c>
+      <c r="P105" s="36">
+        <v>5</v>
+      </c>
+      <c r="Q105" s="37">
+        <v>61331.657399999996</v>
+      </c>
+      <c r="S105" s="8">
+        <v>1000</v>
+      </c>
+      <c r="T105" s="8">
+        <f>H111</f>
+        <v>79.554299999999984</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A106" s="36">
+        <v>6</v>
+      </c>
+      <c r="B106" s="37">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="D106" s="36">
+        <v>6</v>
+      </c>
+      <c r="E106" s="37">
+        <v>0.1618</v>
+      </c>
+      <c r="G106" s="36">
+        <v>6</v>
+      </c>
+      <c r="H106" s="37">
+        <v>73.546000000000006</v>
+      </c>
+      <c r="J106" s="36">
+        <v>6</v>
+      </c>
+      <c r="K106" s="37">
+        <v>1565.1421</v>
+      </c>
+      <c r="M106" s="36">
+        <v>6</v>
+      </c>
+      <c r="N106" s="37">
+        <v>11903.4175</v>
+      </c>
+      <c r="P106" s="36">
+        <v>6</v>
+      </c>
+      <c r="Q106" s="37">
+        <v>57481.728600000002</v>
+      </c>
+      <c r="S106" s="12">
+        <v>5000</v>
+      </c>
+      <c r="T106" s="12">
+        <f>K111</f>
+        <v>1950.5017</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A107" s="36">
+        <v>7</v>
+      </c>
+      <c r="B107" s="37">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D107" s="36">
+        <v>7</v>
+      </c>
+      <c r="E107" s="37">
+        <v>0.16520000000000001</v>
+      </c>
+      <c r="G107" s="36">
+        <v>7</v>
+      </c>
+      <c r="H107" s="37">
+        <v>85.463999999999999</v>
+      </c>
+      <c r="J107" s="36">
+        <v>7</v>
+      </c>
+      <c r="K107" s="37">
+        <v>1838.1594</v>
+      </c>
+      <c r="M107" s="36">
+        <v>7</v>
+      </c>
+      <c r="N107" s="37">
+        <v>12369.947899999999</v>
+      </c>
+      <c r="P107" s="36">
+        <v>7</v>
+      </c>
+      <c r="Q107" s="37">
+        <v>60121.224099999999</v>
+      </c>
+      <c r="S107" s="8">
+        <v>10000</v>
+      </c>
+      <c r="T107" s="8">
+        <f>N111</f>
+        <v>11241.370299999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A108" s="36">
+        <v>8</v>
+      </c>
+      <c r="B108" s="37">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="D108" s="36">
+        <v>8</v>
+      </c>
+      <c r="E108" s="37">
+        <v>0.16189999999999999</v>
+      </c>
+      <c r="G108" s="36">
+        <v>8</v>
+      </c>
+      <c r="H108" s="37">
+        <v>99.217799999999997</v>
+      </c>
+      <c r="J108" s="36">
+        <v>8</v>
+      </c>
+      <c r="K108" s="37">
+        <v>1796.5134</v>
+      </c>
+      <c r="M108" s="36">
+        <v>8</v>
+      </c>
+      <c r="N108" s="37">
+        <v>11807.3511</v>
+      </c>
+      <c r="P108" s="36">
+        <v>8</v>
+      </c>
+      <c r="Q108" s="37">
+        <v>59423.9974</v>
+      </c>
+      <c r="S108" s="8">
+        <v>20000</v>
+      </c>
+      <c r="T108" s="8">
+        <f>Q111</f>
+        <v>58660.935979999995</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A109" s="36">
+        <v>9</v>
+      </c>
+      <c r="B109" s="37">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="D109" s="36">
+        <v>9</v>
+      </c>
+      <c r="E109" s="37">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="G109" s="36">
+        <v>9</v>
+      </c>
+      <c r="H109" s="37">
+        <v>82.908199999999994</v>
+      </c>
+      <c r="J109" s="36">
+        <v>9</v>
+      </c>
+      <c r="K109" s="37">
+        <v>2139.616</v>
+      </c>
+      <c r="M109" s="36">
+        <v>9</v>
+      </c>
+      <c r="N109" s="37">
+        <v>12727.7762</v>
+      </c>
+      <c r="P109" s="36">
+        <v>9</v>
+      </c>
+      <c r="Q109" s="37">
+        <v>60555.396800000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A110" s="36">
+        <v>10</v>
+      </c>
+      <c r="B110" s="37">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="D110" s="36">
+        <v>10</v>
+      </c>
+      <c r="E110" s="37">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="G110" s="36">
+        <v>10</v>
+      </c>
+      <c r="H110" s="37">
+        <v>125.3449</v>
+      </c>
+      <c r="J110" s="36">
+        <v>10</v>
+      </c>
+      <c r="K110" s="37">
+        <v>1536.5642</v>
+      </c>
+      <c r="M110" s="36">
+        <v>10</v>
+      </c>
+      <c r="N110" s="37">
+        <v>12176.0676</v>
+      </c>
+      <c r="P110" s="36">
+        <v>10</v>
+      </c>
+      <c r="Q110" s="37">
+        <v>61404.218399999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A111" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B111" s="36">
+        <f>AVERAGE(B101:B110)</f>
+        <v>3.0789999999999994E-2</v>
+      </c>
+      <c r="D111" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E111" s="36">
+        <f>AVERAGE(E101:E110)</f>
+        <v>0.27732000000000007</v>
+      </c>
+      <c r="G111" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="H111" s="36">
+        <f>AVERAGE(H101:H110)</f>
+        <v>79.554299999999984</v>
+      </c>
+      <c r="J111" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K111" s="36">
+        <f>AVERAGE(K101:K110)</f>
+        <v>1950.5017</v>
+      </c>
+      <c r="M111" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="N111" s="36">
+        <f>AVERAGE(N101:N110)</f>
+        <v>11241.370299999999</v>
+      </c>
+      <c r="P111" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q111" s="36">
+        <f>AVERAGE(Q101:Q110)</f>
+        <v>58660.935979999995</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="56">
+    <mergeCell ref="S101:T101"/>
     <mergeCell ref="S87:T87"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="P99:Q99"/>
     <mergeCell ref="P71:Q71"/>
     <mergeCell ref="S73:T73"/>
     <mergeCell ref="A85:B85"/>
@@ -11408,8 +12963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E1DFA1C-B479-9845-B834-AC124B3DC7B7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added timings for SelectionSort method
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissasedgwick/Projects/Makers/Week_10/algorithmic-complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3628FBBA-79F4-CC48-A6D0-E9D210B0B9B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EEC9F7-83EA-274F-BD98-28CBA0EFDA73}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-10500" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{0EC00D74-CF7F-6E46-A448-9AC86E039AD3}"/>
   </bookViews>
@@ -17,10 +17,12 @@
     <sheet name="Graphs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.2" hidden="1">Data!$S$103:$S$108</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Data!$T$103:$T$108</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Data!$S$103:$S$108</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Data!$T$103:$T$108</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Data!$S$117:$S$122</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Data!$T$117:$T$122</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Data!$S$117:$S$122</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Data!$T$117:$T$122</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Data!$S$117:$S$122</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Data!$T$117:$T$122</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="60">
   <si>
     <t>Attempt</t>
   </si>
@@ -195,6 +197,24 @@
   <si>
     <t>Own Pairing on List of length 20000</t>
   </si>
+  <si>
+    <t>Own SelectionSort on List of length 10</t>
+  </si>
+  <si>
+    <t>Own SelectionSort on List of length 100</t>
+  </si>
+  <si>
+    <t>Own SelectionSort on List of length 1000</t>
+  </si>
+  <si>
+    <t>Own SelectionSort on List of length 5000</t>
+  </si>
+  <si>
+    <t>Own SelectionSort on List of length 10000</t>
+  </si>
+  <si>
+    <t>Own selectionSort on List of length 20000</t>
+  </si>
 </sst>
 </file>
 
@@ -209,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +281,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF45A8C1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA8C157"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -392,6 +418,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,6 +431,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA8C157"/>
       <color rgb="FF45A8C1"/>
       <color rgb="FF41A08E"/>
       <color rgb="FFBE77FF"/>
@@ -3287,6 +3319,367 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SelectionSort -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Own Method</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$S$117:$S$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$T$117:$T$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.4270000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7870000000000014E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5001399999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.096320000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>238.96025999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>952.59510999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B5CD-C140-A129-EBC0762EBCCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1689861632"/>
+        <c:axId val="1689863312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1689861632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1689863312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1689863312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1689861632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3607,6 +4000,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -7374,6 +7807,544 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8217,6 +9188,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4BB46C8-FCC3-B54B-BE74-0DB253718367}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8517,10 +9526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D4128A-2966-F54D-A276-45E672D85F83}">
-  <dimension ref="A1:T111"/>
+  <dimension ref="A1:T125"/>
   <sheetViews>
-    <sheetView topLeftCell="D78" workbookViewId="0">
-      <selection activeCell="S103" sqref="S103:T108"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="S117" sqref="S117:T122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12356,7 +13365,7 @@
         <v>34.433230000000002</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="35" t="s">
         <v>48</v>
       </c>
@@ -12896,9 +13905,556 @@
         <v>58660.935979999995</v>
       </c>
     </row>
+    <row r="113" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B113" s="38"/>
+      <c r="D113" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E113" s="38"/>
+      <c r="G113" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H113" s="38"/>
+      <c r="J113" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="K113" s="38"/>
+      <c r="M113" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="N113" s="38"/>
+      <c r="P113" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q113" s="38"/>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A114" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G114" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="H114" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="J114" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K114" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="M114" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N114" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="P114" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q114" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A115" s="39">
+        <v>1</v>
+      </c>
+      <c r="B115" s="40">
+        <v>0.30220000000000002</v>
+      </c>
+      <c r="D115" s="39">
+        <v>1</v>
+      </c>
+      <c r="E115" s="40">
+        <v>0.35010000000000002</v>
+      </c>
+      <c r="G115" s="39">
+        <v>1</v>
+      </c>
+      <c r="H115" s="40">
+        <v>2.9371999999999998</v>
+      </c>
+      <c r="J115" s="39">
+        <v>1</v>
+      </c>
+      <c r="K115" s="40">
+        <v>60.5092</v>
+      </c>
+      <c r="M115" s="39">
+        <v>1</v>
+      </c>
+      <c r="N115" s="40">
+        <v>236.05789999999999</v>
+      </c>
+      <c r="P115" s="39">
+        <v>1</v>
+      </c>
+      <c r="Q115" s="40">
+        <v>951.4819</v>
+      </c>
+      <c r="S115" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="T115" s="24"/>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A116" s="39">
+        <v>2</v>
+      </c>
+      <c r="B116" s="40">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="D116" s="39">
+        <v>2</v>
+      </c>
+      <c r="E116" s="40">
+        <v>3.7199999999999997E-2</v>
+      </c>
+      <c r="G116" s="39">
+        <v>2</v>
+      </c>
+      <c r="H116" s="40">
+        <v>2.5051999999999999</v>
+      </c>
+      <c r="J116" s="39">
+        <v>2</v>
+      </c>
+      <c r="K116" s="40">
+        <v>58.974800000000002</v>
+      </c>
+      <c r="M116" s="39">
+        <v>2</v>
+      </c>
+      <c r="N116" s="40">
+        <v>238.81110000000001</v>
+      </c>
+      <c r="P116" s="39">
+        <v>2</v>
+      </c>
+      <c r="Q116" s="40">
+        <v>950.12990000000002</v>
+      </c>
+      <c r="S116" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T116" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A117" s="39">
+        <v>3</v>
+      </c>
+      <c r="B117" s="40">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="D117" s="39">
+        <v>3</v>
+      </c>
+      <c r="E117" s="40">
+        <v>3.61E-2</v>
+      </c>
+      <c r="G117" s="39">
+        <v>3</v>
+      </c>
+      <c r="H117" s="40">
+        <v>2.4041999999999999</v>
+      </c>
+      <c r="J117" s="39">
+        <v>3</v>
+      </c>
+      <c r="K117" s="40">
+        <v>59.273000000000003</v>
+      </c>
+      <c r="M117" s="39">
+        <v>3</v>
+      </c>
+      <c r="N117" s="40">
+        <v>236.35339999999999</v>
+      </c>
+      <c r="P117" s="39">
+        <v>3</v>
+      </c>
+      <c r="Q117" s="40">
+        <v>947.00869999999998</v>
+      </c>
+      <c r="S117" s="8">
+        <v>10</v>
+      </c>
+      <c r="T117" s="8">
+        <f>B125</f>
+        <v>3.4270000000000002E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A118" s="39">
+        <v>4</v>
+      </c>
+      <c r="B118" s="40">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="D118" s="39">
+        <v>4</v>
+      </c>
+      <c r="E118" s="40">
+        <v>3.4599999999999999E-2</v>
+      </c>
+      <c r="G118" s="39">
+        <v>4</v>
+      </c>
+      <c r="H118" s="40">
+        <v>2.3936999999999999</v>
+      </c>
+      <c r="J118" s="39">
+        <v>4</v>
+      </c>
+      <c r="K118" s="40">
+        <v>61.451700000000002</v>
+      </c>
+      <c r="M118" s="39">
+        <v>4</v>
+      </c>
+      <c r="N118" s="40">
+        <v>241.32669999999999</v>
+      </c>
+      <c r="P118" s="39">
+        <v>4</v>
+      </c>
+      <c r="Q118" s="40">
+        <v>945.6155</v>
+      </c>
+      <c r="S118" s="8">
+        <v>100</v>
+      </c>
+      <c r="T118" s="8">
+        <f>E125</f>
+        <v>6.7870000000000014E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A119" s="39">
+        <v>5</v>
+      </c>
+      <c r="B119" s="40">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="D119" s="39">
+        <v>5</v>
+      </c>
+      <c r="E119" s="40">
+        <v>3.78E-2</v>
+      </c>
+      <c r="G119" s="39">
+        <v>5</v>
+      </c>
+      <c r="H119" s="40">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="J119" s="39">
+        <v>5</v>
+      </c>
+      <c r="K119" s="40">
+        <v>60.056199999999997</v>
+      </c>
+      <c r="M119" s="39">
+        <v>5</v>
+      </c>
+      <c r="N119" s="40">
+        <v>243.0386</v>
+      </c>
+      <c r="P119" s="39">
+        <v>5</v>
+      </c>
+      <c r="Q119" s="40">
+        <v>950.47879999999998</v>
+      </c>
+      <c r="S119" s="8">
+        <v>1000</v>
+      </c>
+      <c r="T119" s="8">
+        <f>H125</f>
+        <v>2.5001399999999996</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A120" s="39">
+        <v>6</v>
+      </c>
+      <c r="B120" s="40">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="D120" s="39">
+        <v>6</v>
+      </c>
+      <c r="E120" s="40">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="G120" s="39">
+        <v>6</v>
+      </c>
+      <c r="H120" s="40">
+        <v>2.3832</v>
+      </c>
+      <c r="J120" s="39">
+        <v>6</v>
+      </c>
+      <c r="K120" s="40">
+        <v>63.016800000000003</v>
+      </c>
+      <c r="M120" s="39">
+        <v>6</v>
+      </c>
+      <c r="N120" s="40">
+        <v>239.94489999999999</v>
+      </c>
+      <c r="P120" s="39">
+        <v>6</v>
+      </c>
+      <c r="Q120" s="40">
+        <v>951.0498</v>
+      </c>
+      <c r="S120" s="12">
+        <v>5000</v>
+      </c>
+      <c r="T120" s="12">
+        <f>K125</f>
+        <v>60.096320000000006</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A121" s="39">
+        <v>7</v>
+      </c>
+      <c r="B121" s="40">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="D121" s="39">
+        <v>7</v>
+      </c>
+      <c r="E121" s="40">
+        <v>3.6200000000000003E-2</v>
+      </c>
+      <c r="G121" s="39">
+        <v>7</v>
+      </c>
+      <c r="H121" s="40">
+        <v>2.4317000000000002</v>
+      </c>
+      <c r="J121" s="39">
+        <v>7</v>
+      </c>
+      <c r="K121" s="40">
+        <v>58.506999999999998</v>
+      </c>
+      <c r="M121" s="39">
+        <v>7</v>
+      </c>
+      <c r="N121" s="40">
+        <v>239.19040000000001</v>
+      </c>
+      <c r="P121" s="39">
+        <v>7</v>
+      </c>
+      <c r="Q121" s="40">
+        <v>952.8818</v>
+      </c>
+      <c r="S121" s="8">
+        <v>10000</v>
+      </c>
+      <c r="T121" s="8">
+        <f>N125</f>
+        <v>238.96025999999998</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A122" s="39">
+        <v>8</v>
+      </c>
+      <c r="B122" s="40">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="D122" s="39">
+        <v>8</v>
+      </c>
+      <c r="E122" s="40">
+        <v>3.56E-2</v>
+      </c>
+      <c r="G122" s="39">
+        <v>8</v>
+      </c>
+      <c r="H122" s="40">
+        <v>2.5326</v>
+      </c>
+      <c r="J122" s="39">
+        <v>8</v>
+      </c>
+      <c r="K122" s="40">
+        <v>58.842199999999998</v>
+      </c>
+      <c r="M122" s="39">
+        <v>8</v>
+      </c>
+      <c r="N122" s="40">
+        <v>242.90809999999999</v>
+      </c>
+      <c r="P122" s="39">
+        <v>8</v>
+      </c>
+      <c r="Q122" s="40">
+        <v>958.99879999999996</v>
+      </c>
+      <c r="S122" s="8">
+        <v>20000</v>
+      </c>
+      <c r="T122" s="8">
+        <f>Q125</f>
+        <v>952.59510999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A123" s="39">
+        <v>9</v>
+      </c>
+      <c r="B123" s="40">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="D123" s="39">
+        <v>9</v>
+      </c>
+      <c r="E123" s="40">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="G123" s="39">
+        <v>9</v>
+      </c>
+      <c r="H123" s="40">
+        <v>2.4386999999999999</v>
+      </c>
+      <c r="J123" s="39">
+        <v>9</v>
+      </c>
+      <c r="K123" s="40">
+        <v>59.386600000000001</v>
+      </c>
+      <c r="M123" s="39">
+        <v>9</v>
+      </c>
+      <c r="N123" s="40">
+        <v>236.32050000000001</v>
+      </c>
+      <c r="P123" s="39">
+        <v>9</v>
+      </c>
+      <c r="Q123" s="40">
+        <v>963.25779999999997</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A124" s="39">
+        <v>10</v>
+      </c>
+      <c r="B124" s="40">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="D124" s="39">
+        <v>10</v>
+      </c>
+      <c r="E124" s="40">
+        <v>3.5700000000000003E-2</v>
+      </c>
+      <c r="G124" s="39">
+        <v>10</v>
+      </c>
+      <c r="H124" s="40">
+        <v>2.4849000000000001</v>
+      </c>
+      <c r="J124" s="39">
+        <v>10</v>
+      </c>
+      <c r="K124" s="40">
+        <v>60.945700000000002</v>
+      </c>
+      <c r="M124" s="39">
+        <v>10</v>
+      </c>
+      <c r="N124" s="40">
+        <v>235.65100000000001</v>
+      </c>
+      <c r="P124" s="39">
+        <v>10</v>
+      </c>
+      <c r="Q124" s="40">
+        <v>955.04809999999998</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A125" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B125" s="39">
+        <f>AVERAGE(B115:B124)</f>
+        <v>3.4270000000000002E-2</v>
+      </c>
+      <c r="D125" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E125" s="39">
+        <f>AVERAGE(E115:E124)</f>
+        <v>6.7870000000000014E-2</v>
+      </c>
+      <c r="G125" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H125" s="39">
+        <f>AVERAGE(H115:H124)</f>
+        <v>2.5001399999999996</v>
+      </c>
+      <c r="J125" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="K125" s="39">
+        <f>AVERAGE(K115:K124)</f>
+        <v>60.096320000000006</v>
+      </c>
+      <c r="M125" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="N125" s="39">
+        <f>AVERAGE(N115:N124)</f>
+        <v>238.96025999999998</v>
+      </c>
+      <c r="P125" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q125" s="39">
+        <f>AVERAGE(Q115:Q124)</f>
+        <v>952.59510999999998</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="63">
+    <mergeCell ref="S115:T115"/>
     <mergeCell ref="S101:T101"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="J113:K113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="P113:Q113"/>
     <mergeCell ref="S87:T87"/>
     <mergeCell ref="A99:B99"/>
     <mergeCell ref="D99:E99"/>
@@ -12964,7 +14520,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+      <selection activeCell="X42" sqref="X42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added timings for QuickSort method
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -8,21 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissasedgwick/Projects/Makers/Week_10/algorithmic-complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EEC9F7-83EA-274F-BD98-28CBA0EFDA73}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21319CA9-9379-8B4B-A0E1-23FE1561FFBB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-10500" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{0EC00D74-CF7F-6E46-A448-9AC86E039AD3}"/>
+    <workbookView xWindow="-38400" yWindow="-10500" windowWidth="38400" windowHeight="21140" xr2:uid="{0EC00D74-CF7F-6E46-A448-9AC86E039AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Graphs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.2" hidden="1">Data!$S$117:$S$122</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Data!$T$117:$T$122</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Data!$S$117:$S$122</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Data!$T$117:$T$122</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Data!$S$117:$S$122</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Data!$T$117:$T$122</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Data!$S$131:$S$136</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Data!$T$131:$T$136</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Data!$S$131:$S$136</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Data!$T$131:$T$136</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="60">
   <si>
     <t>Attempt</t>
   </si>
@@ -229,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,6 +285,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA8C157"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC14378"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -423,6 +427,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,6 +440,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC14378"/>
       <color rgb="FFA8C157"/>
       <color rgb="FF45A8C1"/>
       <color rgb="FF41A08E"/>
@@ -757,6 +767,367 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="805063231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> QuickSort</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Own Method</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$S$131:$S$136</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$T$131:$T$136</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.0030000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15040000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.45512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.598469999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>169.47223999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>697.59612000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B461-C346-A553-50351C466858}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1689935584"/>
+        <c:axId val="1689937264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1689935584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1689937264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1689937264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1689935584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3720,6 +4091,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4041,6 +4452,544 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9226,6 +10175,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE0899B4-FBC1-474A-8A5F-05AFAD3BD8DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9526,10 +10513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D4128A-2966-F54D-A276-45E672D85F83}">
-  <dimension ref="A1:T125"/>
+  <dimension ref="A1:T139"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="S117" sqref="S117:T122"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="J136" sqref="J136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14445,9 +15432,556 @@
         <v>952.59510999999998</v>
       </c>
     </row>
+    <row r="127" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B127" s="41"/>
+      <c r="D127" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="E127" s="41"/>
+      <c r="G127" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="H127" s="41"/>
+      <c r="J127" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="K127" s="41"/>
+      <c r="M127" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="N127" s="41"/>
+      <c r="P127" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q127" s="41"/>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A128" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D128" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E128" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G128" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="H128" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="J128" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="K128" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="M128" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="N128" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="P128" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A129" s="42">
+        <v>1</v>
+      </c>
+      <c r="B129" s="43">
+        <v>0.629</v>
+      </c>
+      <c r="D129" s="42">
+        <v>1</v>
+      </c>
+      <c r="E129" s="43">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="G129" s="42">
+        <v>1</v>
+      </c>
+      <c r="H129" s="43">
+        <v>3.3662000000000001</v>
+      </c>
+      <c r="J129" s="42">
+        <v>1</v>
+      </c>
+      <c r="K129" s="43">
+        <v>50.9771</v>
+      </c>
+      <c r="M129" s="42">
+        <v>1</v>
+      </c>
+      <c r="N129" s="43">
+        <v>176.70869999999999</v>
+      </c>
+      <c r="P129" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q129" s="43">
+        <v>744.95529999999997</v>
+      </c>
+      <c r="S129" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="T129" s="24"/>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A130" s="42">
+        <v>2</v>
+      </c>
+      <c r="B130" s="43">
+        <v>7.6E-3</v>
+      </c>
+      <c r="D130" s="42">
+        <v>2</v>
+      </c>
+      <c r="E130" s="43">
+        <v>9.3899999999999997E-2</v>
+      </c>
+      <c r="G130" s="42">
+        <v>2</v>
+      </c>
+      <c r="H130" s="43">
+        <v>3.1669999999999998</v>
+      </c>
+      <c r="J130" s="42">
+        <v>2</v>
+      </c>
+      <c r="K130" s="43">
+        <v>53.4724</v>
+      </c>
+      <c r="M130" s="42">
+        <v>2</v>
+      </c>
+      <c r="N130" s="43">
+        <v>169.73570000000001</v>
+      </c>
+      <c r="P130" s="42">
+        <v>2</v>
+      </c>
+      <c r="Q130" s="43">
+        <v>678.77639999999997</v>
+      </c>
+      <c r="S130" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T130" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A131" s="42">
+        <v>3</v>
+      </c>
+      <c r="B131" s="43">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="D131" s="42">
+        <v>3</v>
+      </c>
+      <c r="E131" s="43">
+        <v>9.9900000000000003E-2</v>
+      </c>
+      <c r="G131" s="42">
+        <v>3</v>
+      </c>
+      <c r="H131" s="43">
+        <v>2.9315000000000002</v>
+      </c>
+      <c r="J131" s="42">
+        <v>3</v>
+      </c>
+      <c r="K131" s="43">
+        <v>45.404299999999999</v>
+      </c>
+      <c r="M131" s="42">
+        <v>3</v>
+      </c>
+      <c r="N131" s="43">
+        <v>178.51230000000001</v>
+      </c>
+      <c r="P131" s="42">
+        <v>3</v>
+      </c>
+      <c r="Q131" s="43">
+        <v>672.99170000000004</v>
+      </c>
+      <c r="S131" s="8">
+        <v>10</v>
+      </c>
+      <c r="T131" s="8">
+        <f>B139</f>
+        <v>7.0030000000000009E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A132" s="42">
+        <v>4</v>
+      </c>
+      <c r="B132" s="43">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D132" s="42">
+        <v>4</v>
+      </c>
+      <c r="E132" s="43">
+        <v>0.11219999999999999</v>
+      </c>
+      <c r="G132" s="42">
+        <v>4</v>
+      </c>
+      <c r="H132" s="43">
+        <v>3.0788000000000002</v>
+      </c>
+      <c r="J132" s="42">
+        <v>4</v>
+      </c>
+      <c r="K132" s="43">
+        <v>50.386400000000002</v>
+      </c>
+      <c r="M132" s="42">
+        <v>4</v>
+      </c>
+      <c r="N132" s="43">
+        <v>169.90029999999999</v>
+      </c>
+      <c r="P132" s="42">
+        <v>4</v>
+      </c>
+      <c r="Q132" s="43">
+        <v>670.78009999999995</v>
+      </c>
+      <c r="S132" s="8">
+        <v>100</v>
+      </c>
+      <c r="T132" s="8">
+        <f>E139</f>
+        <v>0.15040000000000003</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A133" s="42">
+        <v>5</v>
+      </c>
+      <c r="B133" s="43">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="D133" s="42">
+        <v>5</v>
+      </c>
+      <c r="E133" s="43">
+        <v>0.1176</v>
+      </c>
+      <c r="G133" s="42">
+        <v>5</v>
+      </c>
+      <c r="H133" s="43">
+        <v>1.8515999999999999</v>
+      </c>
+      <c r="J133" s="42">
+        <v>5</v>
+      </c>
+      <c r="K133" s="43">
+        <v>58.484699999999997</v>
+      </c>
+      <c r="M133" s="42">
+        <v>5</v>
+      </c>
+      <c r="N133" s="43">
+        <v>155.9923</v>
+      </c>
+      <c r="P133" s="42">
+        <v>5</v>
+      </c>
+      <c r="Q133" s="43">
+        <v>710.98940000000005</v>
+      </c>
+      <c r="S133" s="8">
+        <v>1000</v>
+      </c>
+      <c r="T133" s="8">
+        <f>H139</f>
+        <v>3.45512</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A134" s="42">
+        <v>6</v>
+      </c>
+      <c r="B134" s="43">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="D134" s="42">
+        <v>6</v>
+      </c>
+      <c r="E134" s="43">
+        <v>7.0599999999999996E-2</v>
+      </c>
+      <c r="G134" s="42">
+        <v>6</v>
+      </c>
+      <c r="H134" s="43">
+        <v>9.2151999999999994</v>
+      </c>
+      <c r="J134" s="42">
+        <v>6</v>
+      </c>
+      <c r="K134" s="43">
+        <v>54.6449</v>
+      </c>
+      <c r="M134" s="42">
+        <v>6</v>
+      </c>
+      <c r="N134" s="43">
+        <v>163.82220000000001</v>
+      </c>
+      <c r="P134" s="42">
+        <v>6</v>
+      </c>
+      <c r="Q134" s="43">
+        <v>691.5652</v>
+      </c>
+      <c r="S134" s="12">
+        <v>5000</v>
+      </c>
+      <c r="T134" s="12">
+        <f>K139</f>
+        <v>48.598469999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A135" s="42">
+        <v>7</v>
+      </c>
+      <c r="B135" s="43">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="D135" s="42">
+        <v>7</v>
+      </c>
+      <c r="E135" s="43">
+        <v>6.1600000000000002E-2</v>
+      </c>
+      <c r="G135" s="42">
+        <v>7</v>
+      </c>
+      <c r="H135" s="43">
+        <v>1.7911999999999999</v>
+      </c>
+      <c r="J135" s="42">
+        <v>7</v>
+      </c>
+      <c r="K135" s="43">
+        <v>37.795999999999999</v>
+      </c>
+      <c r="M135" s="42">
+        <v>7</v>
+      </c>
+      <c r="N135" s="43">
+        <v>161.28460000000001</v>
+      </c>
+      <c r="P135" s="42">
+        <v>7</v>
+      </c>
+      <c r="Q135" s="43">
+        <v>716.18079999999998</v>
+      </c>
+      <c r="S135" s="8">
+        <v>10000</v>
+      </c>
+      <c r="T135" s="8">
+        <f>N139</f>
+        <v>169.47223999999997</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A136" s="42">
+        <v>8</v>
+      </c>
+      <c r="B136" s="43">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="D136" s="42">
+        <v>8</v>
+      </c>
+      <c r="E136" s="43">
+        <v>6.8199999999999997E-2</v>
+      </c>
+      <c r="G136" s="42">
+        <v>8</v>
+      </c>
+      <c r="H136" s="43">
+        <v>1.8486</v>
+      </c>
+      <c r="J136" s="42">
+        <v>8</v>
+      </c>
+      <c r="K136" s="43">
+        <v>37.604199999999999</v>
+      </c>
+      <c r="M136" s="42">
+        <v>8</v>
+      </c>
+      <c r="N136" s="43">
+        <v>170.13159999999999</v>
+      </c>
+      <c r="P136" s="42">
+        <v>8</v>
+      </c>
+      <c r="Q136" s="43">
+        <v>693.47130000000004</v>
+      </c>
+      <c r="S136" s="8">
+        <v>20000</v>
+      </c>
+      <c r="T136" s="8">
+        <f>Q139</f>
+        <v>697.59612000000004</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A137" s="42">
+        <v>9</v>
+      </c>
+      <c r="B137" s="43">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D137" s="42">
+        <v>9</v>
+      </c>
+      <c r="E137" s="43">
+        <v>6.3899999999999998E-2</v>
+      </c>
+      <c r="G137" s="42">
+        <v>9</v>
+      </c>
+      <c r="H137" s="43">
+        <v>1.9297</v>
+      </c>
+      <c r="J137" s="42">
+        <v>9</v>
+      </c>
+      <c r="K137" s="43">
+        <v>44.892299999999999</v>
+      </c>
+      <c r="M137" s="42">
+        <v>9</v>
+      </c>
+      <c r="N137" s="43">
+        <v>175.46209999999999</v>
+      </c>
+      <c r="P137" s="42">
+        <v>9</v>
+      </c>
+      <c r="Q137" s="43">
+        <v>694.5865</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A138" s="42">
+        <v>10</v>
+      </c>
+      <c r="B138" s="43">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="D138" s="42">
+        <v>10</v>
+      </c>
+      <c r="E138" s="43">
+        <v>6.0100000000000001E-2</v>
+      </c>
+      <c r="G138" s="42">
+        <v>10</v>
+      </c>
+      <c r="H138" s="43">
+        <v>5.3714000000000004</v>
+      </c>
+      <c r="J138" s="42">
+        <v>10</v>
+      </c>
+      <c r="K138" s="43">
+        <v>52.322400000000002</v>
+      </c>
+      <c r="M138" s="42">
+        <v>10</v>
+      </c>
+      <c r="N138" s="43">
+        <v>173.17259999999999</v>
+      </c>
+      <c r="P138" s="42">
+        <v>10</v>
+      </c>
+      <c r="Q138" s="43">
+        <v>701.66449999999998</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A139" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B139" s="42">
+        <f>AVERAGE(B129:B138)</f>
+        <v>7.0030000000000009E-2</v>
+      </c>
+      <c r="D139" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E139" s="42">
+        <f>AVERAGE(E129:E138)</f>
+        <v>0.15040000000000003</v>
+      </c>
+      <c r="G139" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="H139" s="42">
+        <f>AVERAGE(H129:H138)</f>
+        <v>3.45512</v>
+      </c>
+      <c r="J139" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="K139" s="42">
+        <f>AVERAGE(K129:K138)</f>
+        <v>48.598469999999999</v>
+      </c>
+      <c r="M139" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="N139" s="42">
+        <f>AVERAGE(N129:N138)</f>
+        <v>169.47223999999997</v>
+      </c>
+      <c r="P139" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q139" s="42">
+        <f>AVERAGE(Q129:Q138)</f>
+        <v>697.59612000000004</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="63">
+  <mergeCells count="70">
+    <mergeCell ref="S129:T129"/>
     <mergeCell ref="S115:T115"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="G127:H127"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="M127:N127"/>
+    <mergeCell ref="P127:Q127"/>
     <mergeCell ref="S101:T101"/>
     <mergeCell ref="A113:B113"/>
     <mergeCell ref="D113:E113"/>
@@ -14519,8 +16053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E1DFA1C-B479-9845-B834-AC124B3DC7B7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="X42" sqref="X42"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>